<commit_message>
update of unifloc exapmles - all examples should be ok for now
</commit_message>
<xml_diff>
--- a/examples/ex120.GLV.xlsx
+++ b/examples/ex120.GLV.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\unifloc\unifloc_vba\examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\unifloc\unifloc_vba\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC14448-6204-4727-ABE3-762A70A8CEA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9BF1AED-7D89-4E53-A6C4-24099CA4DC29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{7F603498-48FA-40A8-AB9B-D5E4C9CE020B}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{7F603498-48FA-40A8-AB9B-D5E4C9CE020B}"/>
   </bookViews>
   <sheets>
     <sheet name="Клапана" sheetId="2" r:id="rId1"/>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="45">
   <si>
     <t>Клапан</t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t>Расчет параметров  газлифтных клапанов</t>
+  </si>
+  <si>
+    <t>0,8</t>
   </si>
 </sst>
 </file>
@@ -536,6 +539,30 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="9" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -561,33 +588,9 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="3" borderId="9" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2" xfId="1" xr:uid="{59DE2439-BB31-4F47-9019-227E568A9073}"/>
     <cellStyle name="Финансовый 2" xfId="2" xr:uid="{76448D99-8040-4132-8D13-109A8AFF0A7E}"/>
   </cellStyles>
@@ -621,7 +624,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -680,7 +683,7 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>50.000325594155143</c:v>
+                  <c:v>49.952452966948883</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -692,7 +695,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>14325.967142632906</c:v>
+                  <c:v>14326.055531312555</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -879,157 +882,157 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
                 <c:pt idx="0">
-                  <c:v>15132.29321842874</c:v>
+                  <c:v>15132.293218428747</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15132.293527067584</c:v>
+                  <c:v>15132.375521433616</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15132.293723711133</c:v>
+                  <c:v>15132.293723711138</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15132.293689852137</c:v>
+                  <c:v>15132.351640856588</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15132.293757570382</c:v>
+                  <c:v>15132.380465611186</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15132.293394886816</c:v>
+                  <c:v>15132.306703253296</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15132.29376277928</c:v>
+                  <c:v>15132.315932744956</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15132.293339540312</c:v>
+                  <c:v>15132.364500612437</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>15132.293458698452</c:v>
+                  <c:v>15132.328287327928</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>15132.293406607414</c:v>
+                  <c:v>15132.311802105083</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>15132.293611715582</c:v>
+                  <c:v>15132.428086533779</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>15132.293837008969</c:v>
+                  <c:v>15132.347992396371</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>15132.293614319904</c:v>
+                  <c:v>15132.293614319911</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>15132.293208010429</c:v>
+                  <c:v>15132.293208010435</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>15132.293645574835</c:v>
+                  <c:v>15132.293645574842</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15132.293499720034</c:v>
+                  <c:v>15132.293499720039</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>15132.293467814217</c:v>
+                  <c:v>15132.31637660822</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>15132.293882588816</c:v>
+                  <c:v>15132.406299383623</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>15132.293598692951</c:v>
+                  <c:v>15132.293598692959</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>15132.293890402292</c:v>
+                  <c:v>15132.293890402299</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>15132.293775802425</c:v>
+                  <c:v>15132.293775802431</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>15132.293773197591</c:v>
+                  <c:v>15132.330117306123</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>15132.293308285638</c:v>
+                  <c:v>15132.339364156793</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>15132.293396840249</c:v>
+                  <c:v>15132.444305090065</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>15132.293541392761</c:v>
+                  <c:v>15132.593044874915</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>15132.293252287735</c:v>
+                  <c:v>15132.436227065908</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>15132.293714595367</c:v>
+                  <c:v>15132.317098549966</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>15132.29391644781</c:v>
+                  <c:v>15132.421149090058</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>15123.567390728282</c:v>
+                  <c:v>15123.567390728287</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>15087.810103088721</c:v>
+                  <c:v>15087.823257771033</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>15024.040340821331</c:v>
+                  <c:v>15024.088805923846</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>14931.698783899501</c:v>
+                  <c:v>14931.930165945385</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>14810.07554969816</c:v>
+                  <c:v>14810.117273269569</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>14658.28511717961</c:v>
+                  <c:v>14658.285117179616</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>14475.242195036955</c:v>
+                  <c:v>14475.242195036961</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>14259.626207372432</c:v>
+                  <c:v>14259.812715443462</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>14009.829781204478</c:v>
+                  <c:v>14009.855395414645</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>13723.900434714098</c:v>
+                  <c:v>13723.985036855227</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>13399.451233769601</c:v>
+                  <c:v>13399.611072142128</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>13033.546109785839</c:v>
+                  <c:v>13033.611809348726</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>12622.531064812889</c:v>
+                  <c:v>12622.558699543064</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>12161.797122579219</c:v>
+                  <c:v>12161.862989000681</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>11645.419699120408</c:v>
+                  <c:v>11645.470475847967</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>11065.595095987857</c:v>
+                  <c:v>11065.613139281118</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>10411.724986497131</c:v>
+                  <c:v>10411.738924275027</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>9668.8049835757247</c:v>
+                  <c:v>9668.8968073502783</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>8814.3645636878318</c:v>
+                  <c:v>8814.4424417758291</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>7811.9276946842756</c:v>
+                  <c:v>7811.9570849652991</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>6594.3921634374583</c:v>
+                  <c:v>6594.3921634374619</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>5007.3142166950001</c:v>
+                  <c:v>5007.3796364780646</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>2405.9714599975982</c:v>
+                  <c:v>2406.0122810436478</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1139,7 +1142,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1210,7 +1213,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>14325.967142632906</c:v>
+                  <c:v>14326.055531312555</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1633,94 +1636,94 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>12794.396624196695</c:v>
+                  <c:v>12794.551782045031</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>13282.150153055929</c:v>
+                  <c:v>13282.335488606182</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>13749.423910087005</c:v>
+                  <c:v>13749.522711983491</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>14198.269666518319</c:v>
+                  <c:v>14198.306787296195</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>14630.414688406485</c:v>
+                  <c:v>14630.446737999669</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>15047.328305168016</c:v>
+                  <c:v>15047.369694955658</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>15450.274923663121</c:v>
+                  <c:v>15450.274923663128</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>15840.351571150621</c:v>
+                  <c:v>15844.147396689053</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>16218.518742724227</c:v>
+                  <c:v>16218.518742724234</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>16585.622292462373</c:v>
+                  <c:v>16585.680858167587</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>16942.411442652079</c:v>
+                  <c:v>16942.411442652083</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>17289.55520135515</c:v>
+                  <c:v>17289.614197050938</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>17627.654061073394</c:v>
+                  <c:v>17627.680677787979</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>17957.247774838354</c:v>
+                  <c:v>17957.346134896223</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>18278.825823409399</c:v>
+                  <c:v>18278.854772828065</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>18592.83192811739</c:v>
+                  <c:v>18593.504749915024</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>18899.671325158339</c:v>
+                  <c:v>18899.6877139922</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>19199.715657092231</c:v>
+                  <c:v>19199.901980928051</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>19496.426925926004</c:v>
+                  <c:v>19496.48142348669</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>19793.138845896636</c:v>
+                  <c:v>19793.154075247352</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>20089.850497598603</c:v>
+                  <c:v>20089.929004556132</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>20386.562100465428</c:v>
+                  <c:v>20386.596363812845</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>20683.273903882506</c:v>
+                  <c:v>20683.372066720633</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>20979.985094579846</c:v>
+                  <c:v>20980.03300848461</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>21276.697456021215</c:v>
+                  <c:v>21276.766733582681</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>21573.408411006203</c:v>
+                  <c:v>21573.469266751661</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>21870.119931178731</c:v>
+                  <c:v>21870.245663779282</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>22166.831814685807</c:v>
+                  <c:v>22166.875820776397</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>22463.543672147567</c:v>
+                  <c:v>22463.773442080615</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>22760.255329709704</c:v>
+                  <c:v>22760.290125397136</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2141,82 +2144,82 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>14630.414688406485</c:v>
+                  <c:v>14630.446737999669</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>15047.328305168016</c:v>
+                  <c:v>15047.369694955658</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>15450.274923663121</c:v>
+                  <c:v>15450.274923663128</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>15840.351571150621</c:v>
+                  <c:v>15844.147396689053</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>16218.518742724227</c:v>
+                  <c:v>16218.518742724234</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>16585.622292462373</c:v>
+                  <c:v>16585.680858167587</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>16942.411442652079</c:v>
+                  <c:v>16942.411442652083</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>17289.55520135515</c:v>
+                  <c:v>17289.614197050938</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>17627.654061073394</c:v>
+                  <c:v>17627.680677787979</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>17957.247774838354</c:v>
+                  <c:v>17957.346134896223</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>18278.825823409399</c:v>
+                  <c:v>18278.854772828065</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>18592.83192811739</c:v>
+                  <c:v>18593.504749915024</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>18899.671325158339</c:v>
+                  <c:v>18899.6877139922</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>19199.715657092231</c:v>
+                  <c:v>19199.901980928051</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>19496.426925926004</c:v>
+                  <c:v>19496.48142348669</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>19793.138845896636</c:v>
+                  <c:v>19793.154075247352</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>20089.850497598603</c:v>
+                  <c:v>20089.929004556132</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>20386.562100465428</c:v>
+                  <c:v>20386.596363812845</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>20683.273903882506</c:v>
+                  <c:v>20683.372066720633</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>20979.985094579846</c:v>
+                  <c:v>20980.03300848461</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>21276.697456021215</c:v>
+                  <c:v>21276.766733582681</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>21573.408411006203</c:v>
+                  <c:v>21573.469266751661</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>21870.119931178731</c:v>
+                  <c:v>21870.245663779282</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>22166.831814685807</c:v>
+                  <c:v>22166.875820776397</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>22463.543672147567</c:v>
+                  <c:v>22463.773442080615</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>22760.255329709704</c:v>
+                  <c:v>22760.290125397136</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2417,8 +2420,11 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Info"/>
     </sheetNames>
@@ -2438,9 +2444,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2478,7 +2484,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2584,7 +2590,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2738,31 +2744,31 @@
   <dimension ref="A1:AD99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.1328125" style="1"/>
+    <col min="1" max="1" width="9.15234375" style="1"/>
     <col min="2" max="2" width="28" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.73046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.69140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="1" customWidth="1"/>
-    <col min="5" max="6" width="9.1328125" style="1"/>
-    <col min="7" max="7" width="11.265625" style="1" customWidth="1"/>
-    <col min="8" max="20" width="9.1328125" style="1"/>
+    <col min="5" max="6" width="9.15234375" style="1"/>
+    <col min="7" max="7" width="20" style="1" customWidth="1"/>
+    <col min="8" max="20" width="9.15234375" style="1"/>
     <col min="21" max="21" width="15" style="1" customWidth="1"/>
-    <col min="22" max="22" width="9.1328125" style="1"/>
+    <col min="22" max="22" width="9.15234375" style="1"/>
     <col min="23" max="23" width="12" style="1" customWidth="1"/>
-    <col min="24" max="24" width="16.73046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.1328125" style="1" customWidth="1"/>
+    <col min="24" max="24" width="16.69140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.15234375" style="1" customWidth="1"/>
     <col min="26" max="26" width="12" style="1" customWidth="1"/>
-    <col min="27" max="27" width="13.86328125" style="1" customWidth="1"/>
-    <col min="28" max="29" width="9.1328125" style="1"/>
-    <col min="30" max="30" width="9.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="16384" width="9.1328125" style="1"/>
+    <col min="27" max="27" width="13.84375" style="1" customWidth="1"/>
+    <col min="28" max="29" width="9.15234375" style="1"/>
+    <col min="30" max="30" width="9.61328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="9.15234375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="38.25" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:30" ht="37.299999999999997" x14ac:dyDescent="0.4">
       <c r="A1" s="22" t="s">
         <v>41</v>
       </c>
@@ -2775,7 +2781,7 @@
       </c>
       <c r="G1" t="str" cm="1">
         <f t="array" ref="G1">[1]!unf_version()</f>
-        <v>7.38</v>
+        <v>7.49</v>
       </c>
       <c r="H1"/>
       <c r="U1" s="1" t="s">
@@ -2809,7 +2815,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:30" ht="14.6" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -2833,7 +2839,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:30" ht="12.9" thickBot="1" x14ac:dyDescent="0.35">
       <c r="U3" s="1" t="s">
         <v>12</v>
       </c>
@@ -2869,13 +2875,13 @@
         <v>4.3841336116910233E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:30" ht="13.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="23" t="s">
+    <row r="4" spans="1:30" ht="12.9" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="25"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="31"/>
       <c r="V4" s="1" t="s">
         <v>13</v>
       </c>
@@ -2908,20 +2914,20 @@
         <v>7.2673639045320468E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:30" ht="14.6" x14ac:dyDescent="0.4">
       <c r="B5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="27"/>
+      <c r="D5" s="33"/>
       <c r="E5" s="7"/>
       <c r="G5" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="14">
-        <v>0.8</v>
+      <c r="H5" s="14" t="s">
+        <v>44</v>
       </c>
       <c r="I5" s="15"/>
       <c r="J5" s="9"/>
@@ -2957,14 +2963,14 @@
         <v>0.10320480997297149</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:30" ht="14.6" x14ac:dyDescent="0.4">
       <c r="B6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="28"/>
+      <c r="D6" s="34"/>
       <c r="E6" s="9"/>
       <c r="G6" s="8" t="s">
         <v>33</v>
@@ -3008,14 +3014,14 @@
         <v>0.20156203063983175</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:30" ht="14.6" x14ac:dyDescent="0.4">
       <c r="B7" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="28"/>
+      <c r="D7" s="34"/>
       <c r="E7" s="9"/>
       <c r="V7" s="1" t="s">
         <v>13</v>
@@ -3049,71 +3055,71 @@
         <v>0.34779971696205947</v>
       </c>
     </row>
-    <row r="8" spans="1:30" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:30" ht="14.6" x14ac:dyDescent="0.4">
       <c r="B8" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="29">
+      <c r="C8" s="35">
         <f>VLOOKUP(C11,W3:AD7,2,0)</f>
         <v>25.4</v>
       </c>
-      <c r="D8" s="29"/>
+      <c r="D8" s="35"/>
       <c r="E8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="X8" s="2"/>
       <c r="Y8" s="2"/>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="X9" s="2"/>
       <c r="Y9" s="2"/>
       <c r="Z9" s="3"/>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
     </row>
-    <row r="11" spans="1:30" ht="13.15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B11" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="32" t="s">
+      <c r="C11" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="32"/>
+      <c r="D11" s="25"/>
       <c r="E11" s="9"/>
       <c r="X11" s="2"/>
       <c r="Y11" s="2"/>
     </row>
-    <row r="12" spans="1:30" ht="13.15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B12" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="33">
+      <c r="C12" s="26">
         <f>VLOOKUP(C11,W3:AD7,4,0)</f>
         <v>7.94</v>
       </c>
-      <c r="D12" s="33"/>
+      <c r="D12" s="26"/>
       <c r="E12" s="9" t="s">
         <v>10</v>
       </c>
       <c r="X12" s="2"/>
       <c r="Y12" s="2"/>
     </row>
-    <row r="13" spans="1:30" ht="13.15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B13" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="33">
+      <c r="C13" s="26">
         <f>VLOOKUP(C11,W3:AD7,6,0)</f>
         <v>0.25805</v>
       </c>
-      <c r="D13" s="33"/>
+      <c r="D13" s="26"/>
       <c r="E13" s="9"/>
       <c r="X13" s="2"/>
       <c r="Y13" s="2"/>
     </row>
-    <row r="14" spans="1:30" ht="13.15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B14" s="8" t="s">
         <v>24</v>
       </c>
@@ -3131,7 +3137,7 @@
       <c r="X14" s="2"/>
       <c r="Y14" s="2"/>
     </row>
-    <row r="15" spans="1:30" ht="13.15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B15" s="8" t="s">
         <v>25</v>
       </c>
@@ -3143,33 +3149,33 @@
       <c r="X15" s="2"/>
       <c r="Y15" s="2"/>
     </row>
-    <row r="16" spans="1:30" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:30" ht="14.6" x14ac:dyDescent="0.4">
       <c r="B16" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="34">
+      <c r="C16" s="27">
         <f>((C14^2+D14^2+C15^2+D15^2))^(0.5)</f>
         <v>4.2426406871192848</v>
       </c>
-      <c r="D16" s="34"/>
+      <c r="D16" s="27"/>
       <c r="E16" s="9"/>
       <c r="X16" s="2"/>
       <c r="Y16" s="2"/>
     </row>
-    <row r="17" spans="2:25" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:25" ht="14.6" x14ac:dyDescent="0.4">
       <c r="B17" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="35">
+      <c r="C17" s="28">
         <f>C16</f>
         <v>4.2426406871192848</v>
       </c>
-      <c r="D17" s="35"/>
+      <c r="D17" s="28"/>
       <c r="E17" s="9"/>
       <c r="X17" s="2"/>
       <c r="Y17" s="2"/>
     </row>
-    <row r="18" spans="2:25" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:25" x14ac:dyDescent="0.3">
       <c r="G18" s="1" t="e" cm="1">
         <f t="array" ref="G18">GLV_p</f>
         <v>#NAME?</v>
@@ -3177,37 +3183,37 @@
       <c r="X18" s="2"/>
       <c r="Y18" s="2"/>
     </row>
-    <row r="19" spans="2:25" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:25" ht="14.6" x14ac:dyDescent="0.4">
       <c r="B19" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="30">
+      <c r="C19" s="23">
         <v>72</v>
       </c>
-      <c r="D19" s="30"/>
+      <c r="D19" s="23"/>
       <c r="E19" s="9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="2:25" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:25" ht="14.6" x14ac:dyDescent="0.4">
       <c r="B20" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="31">
+      <c r="C20" s="24">
         <v>50</v>
       </c>
-      <c r="D20" s="31"/>
+      <c r="D20" s="24"/>
       <c r="E20" s="9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="2:25" ht="13.15" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B21" s="8" t="s">
         <v>29</v>
       </c>
       <c r="C21" s="19">
         <f t="array" ref="C21:D27">TRANSPOSE([1]!GLV_p_vkr_atma(C12,C17,C19,C29,H5,H6,1))</f>
-        <v>50.000325594155143</v>
+        <v>49.952452966948883</v>
       </c>
       <c r="D21" s="1" t="str">
         <v>p_atma</v>
@@ -3218,7 +3224,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="2:25" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:25" x14ac:dyDescent="0.3">
       <c r="C22" s="19">
         <v>72</v>
       </c>
@@ -3226,9 +3232,9 @@
         <v>p_in_atma</v>
       </c>
     </row>
-    <row r="23" spans="2:25" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:25" x14ac:dyDescent="0.3">
       <c r="C23" s="19">
-        <v>70.885775115731576</v>
+        <v>70.861251006900801</v>
       </c>
       <c r="D23" s="1" t="str">
         <v>p_v_atma</v>
@@ -3238,11 +3244,11 @@
       </c>
       <c r="J23" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I23,$H$5,$H$6)/1000</f>
-        <v>15.132293218428741</v>
+        <v>15.132293218428748</v>
       </c>
       <c r="K23" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I23,$H$5,$H$6)</f>
-        <v>15132.29321842874</v>
+        <v>15132.293218428747</v>
       </c>
       <c r="L23" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I23,$C$20,$H$5,$H$6)</f>
@@ -3257,9 +3263,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:25" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:25" x14ac:dyDescent="0.3">
       <c r="C24" s="20">
-        <v>50.000325594155143</v>
+        <v>49.952452966948883</v>
       </c>
       <c r="D24" s="1" t="str">
         <v>p_out_atma</v>
@@ -3270,11 +3276,11 @@
       </c>
       <c r="J24" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I24,$H$5,$H$6)/1000</f>
-        <v>15.132293527067585</v>
+        <v>15.132375521433616</v>
       </c>
       <c r="K24" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I24,$H$5,$H$6)</f>
-        <v>15132.293527067584</v>
+        <v>15132.375521433616</v>
       </c>
       <c r="L24" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I24,$C$20,$H$5,$H$6)</f>
@@ -3289,9 +3295,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:25" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:25" x14ac:dyDescent="0.3">
       <c r="C25" s="18">
-        <v>14325.967142632906</v>
+        <v>14326.055531312555</v>
       </c>
       <c r="D25" s="1" t="str">
         <v>q_gas_sm3day</v>
@@ -3302,11 +3308,11 @@
       </c>
       <c r="J25" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I25,$H$5,$H$6)/1000</f>
-        <v>15.132293723711133</v>
+        <v>15.132293723711138</v>
       </c>
       <c r="K25" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I25,$H$5,$H$6)</f>
-        <v>15132.293723711133</v>
+        <v>15132.293723711138</v>
       </c>
       <c r="L25" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I25,$C$20,$H$5,$H$6)</f>
@@ -3321,7 +3327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:25" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:25" x14ac:dyDescent="0.3">
       <c r="C26" s="1" t="b">
         <v>0</v>
       </c>
@@ -3334,11 +3340,11 @@
       </c>
       <c r="J26" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I26,$H$5,$H$6)/1000</f>
-        <v>15.132293689852137</v>
+        <v>15.132351640856589</v>
       </c>
       <c r="K26" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I26,$H$5,$H$6)</f>
-        <v>15132.293689852137</v>
+        <v>15132.351640856588</v>
       </c>
       <c r="L26" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I26,$C$20,$H$5,$H$6)</f>
@@ -3353,7 +3359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:25" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:25" x14ac:dyDescent="0.3">
       <c r="C27" s="1" t="b">
         <v>0</v>
       </c>
@@ -3366,11 +3372,11 @@
       </c>
       <c r="J27" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I27,$H$5,$H$6)/1000</f>
-        <v>15.132293757570382</v>
+        <v>15.132380465611186</v>
       </c>
       <c r="K27" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I27,$H$5,$H$6)</f>
-        <v>15132.293757570382</v>
+        <v>15132.380465611186</v>
       </c>
       <c r="L27" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I27,$C$20,$H$5,$H$6)</f>
@@ -3385,18 +3391,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:25" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:25" x14ac:dyDescent="0.3">
       <c r="I28" s="1">
         <f t="shared" si="2"/>
         <v>8.0588235294117663</v>
       </c>
       <c r="J28" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I28,$H$5,$H$6)/1000</f>
-        <v>15.132293394886815</v>
+        <v>15.132306703253295</v>
       </c>
       <c r="K28" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I28,$H$5,$H$6)</f>
-        <v>15132.293394886816</v>
+        <v>15132.306703253296</v>
       </c>
       <c r="L28" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I28,$C$20,$H$5,$H$6)</f>
@@ -3411,13 +3417,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:25" ht="13.15" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B29" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C29" s="18">
         <f t="array" ref="C29:D35">TRANSPOSE([1]!GLV_q_gas_vkr_sm3day(C12,C17,C19,C20,H5,H6))</f>
-        <v>14325.967142632906</v>
+        <v>14326.055531312555</v>
       </c>
       <c r="D29" s="1" t="str">
         <v>q_gas_sm3day</v>
@@ -3428,11 +3434,11 @@
       </c>
       <c r="J29" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I29,$H$5,$H$6)/1000</f>
-        <v>15.13229376277928</v>
+        <v>15.132315932744955</v>
       </c>
       <c r="K29" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I29,$H$5,$H$6)</f>
-        <v>15132.29376277928</v>
+        <v>15132.315932744956</v>
       </c>
       <c r="L29" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I29,$C$20,$H$5,$H$6)</f>
@@ -3447,7 +3453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:25" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:25" x14ac:dyDescent="0.3">
       <c r="C30" s="19">
         <v>72</v>
       </c>
@@ -3460,11 +3466,11 @@
       </c>
       <c r="J30" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I30,$H$5,$H$6)/1000</f>
-        <v>15.132293339540313</v>
+        <v>15.132364500612438</v>
       </c>
       <c r="K30" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I30,$H$5,$H$6)</f>
-        <v>15132.293339540312</v>
+        <v>15132.364500612437</v>
       </c>
       <c r="L30" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I30,$C$20,$H$5,$H$6)</f>
@@ -3479,9 +3485,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:25" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:25" x14ac:dyDescent="0.3">
       <c r="C31" s="19">
-        <v>70.885765224695206</v>
+        <v>70.8857512084967</v>
       </c>
       <c r="D31" s="1" t="str">
         <v>pv_atma</v>
@@ -3492,11 +3498,11 @@
       </c>
       <c r="J31" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I31,$H$5,$H$6)/1000</f>
-        <v>15.132293458698452</v>
+        <v>15.132328287327928</v>
       </c>
       <c r="K31" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I31,$H$5,$H$6)</f>
-        <v>15132.293458698452</v>
+        <v>15132.328287327928</v>
       </c>
       <c r="L31" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I31,$C$20,$H$5,$H$6)</f>
@@ -3511,7 +3517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:25" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:25" x14ac:dyDescent="0.3">
       <c r="C32" s="19">
         <v>50</v>
       </c>
@@ -3524,11 +3530,11 @@
       </c>
       <c r="J32" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I32,$H$5,$H$6)/1000</f>
-        <v>15.132293406607413</v>
+        <v>15.132311802105082</v>
       </c>
       <c r="K32" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I32,$H$5,$H$6)</f>
-        <v>15132.293406607414</v>
+        <v>15132.311802105083</v>
       </c>
       <c r="L32" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I32,$C$20,$H$5,$H$6)</f>
@@ -3543,9 +3549,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C33" s="18">
-        <v>14325.967142632906</v>
+        <v>14326.055531312555</v>
       </c>
       <c r="D33" s="1" t="str">
         <v>q_gas_sm3day</v>
@@ -3556,11 +3562,11 @@
       </c>
       <c r="J33" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I33,$H$5,$H$6)/1000</f>
-        <v>15.132293611715582</v>
+        <v>15.132428086533778</v>
       </c>
       <c r="K33" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I33,$H$5,$H$6)</f>
-        <v>15132.293611715582</v>
+        <v>15132.428086533779</v>
       </c>
       <c r="L33" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I33,$C$20,$H$5,$H$6)</f>
@@ -3575,7 +3581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C34" s="18" t="b">
         <v>0</v>
       </c>
@@ -3588,11 +3594,11 @@
       </c>
       <c r="J34" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I34,$H$5,$H$6)/1000</f>
-        <v>15.132293837008969</v>
+        <v>15.132347992396371</v>
       </c>
       <c r="K34" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I34,$H$5,$H$6)</f>
-        <v>15132.293837008969</v>
+        <v>15132.347992396371</v>
       </c>
       <c r="L34" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I34,$C$20,$H$5,$H$6)</f>
@@ -3607,7 +3613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C35" s="1" t="b">
         <v>0</v>
       </c>
@@ -3620,11 +3626,11 @@
       </c>
       <c r="J35" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I35,$H$5,$H$6)/1000</f>
-        <v>15.132293614319904</v>
+        <v>15.132293614319911</v>
       </c>
       <c r="K35" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I35,$H$5,$H$6)</f>
-        <v>15132.293614319904</v>
+        <v>15132.293614319911</v>
       </c>
       <c r="L35" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I35,$C$20,$H$5,$H$6)</f>
@@ -3639,18 +3645,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:14" x14ac:dyDescent="0.3">
       <c r="I36" s="1">
         <f t="shared" si="2"/>
         <v>19.352941176470587</v>
       </c>
       <c r="J36" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I36,$H$5,$H$6)/1000</f>
-        <v>15.132293208010429</v>
+        <v>15.132293208010434</v>
       </c>
       <c r="K36" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I36,$H$5,$H$6)</f>
-        <v>15132.293208010429</v>
+        <v>15132.293208010435</v>
       </c>
       <c r="L36" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I36,$C$20,$H$5,$H$6)</f>
@@ -3665,7 +3671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:14" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:14" ht="14.6" x14ac:dyDescent="0.4">
       <c r="B37" s="8" t="s">
         <v>35</v>
       </c>
@@ -3682,11 +3688,11 @@
       </c>
       <c r="J37" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I37,$H$5,$H$6)/1000</f>
-        <v>15.132293645574835</v>
+        <v>15.132293645574842</v>
       </c>
       <c r="K37" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I37,$H$5,$H$6)</f>
-        <v>15132.293645574835</v>
+        <v>15132.293645574842</v>
       </c>
       <c r="L37" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I37,$C$20,$H$5,$H$6)</f>
@@ -3701,7 +3707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:14" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:14" ht="14.6" x14ac:dyDescent="0.4">
       <c r="B38" s="8" t="s">
         <v>36</v>
       </c>
@@ -3719,11 +3725,11 @@
       </c>
       <c r="J38" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I38,$H$5,$H$6)/1000</f>
-        <v>15.132293499720033</v>
+        <v>15.132293499720038</v>
       </c>
       <c r="K38" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I38,$H$5,$H$6)</f>
-        <v>15132.293499720034</v>
+        <v>15132.293499720039</v>
       </c>
       <c r="L38" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I38,$C$20,$H$5,$H$6)</f>
@@ -3738,7 +3744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:14" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:14" ht="14.6" x14ac:dyDescent="0.4">
       <c r="B39" s="8" t="s">
         <v>37</v>
       </c>
@@ -3759,11 +3765,11 @@
       </c>
       <c r="J39" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I39,$H$5,$H$6)/1000</f>
-        <v>15.132293467814218</v>
+        <v>15.13231637660822</v>
       </c>
       <c r="K39" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I39,$H$5,$H$6)</f>
-        <v>15132.293467814217</v>
+        <v>15132.31637660822</v>
       </c>
       <c r="L39" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I39,$C$20,$H$5,$H$6)</f>
@@ -3778,7 +3784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:14" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:14" ht="14.6" x14ac:dyDescent="0.4">
       <c r="B40" s="8" t="s">
         <v>38</v>
       </c>
@@ -3799,11 +3805,11 @@
       </c>
       <c r="J40" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I40,$H$5,$H$6)/1000</f>
-        <v>15.132293882588815</v>
+        <v>15.132406299383623</v>
       </c>
       <c r="K40" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I40,$H$5,$H$6)</f>
-        <v>15132.293882588816</v>
+        <v>15132.406299383623</v>
       </c>
       <c r="L40" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I40,$C$20,$H$5,$H$6)</f>
@@ -3818,7 +3824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:14" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="41" spans="2:14" ht="14.6" x14ac:dyDescent="0.4">
       <c r="B41" s="8" t="s">
         <v>39</v>
       </c>
@@ -3834,11 +3840,11 @@
       </c>
       <c r="J41" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I41,$H$5,$H$6)/1000</f>
-        <v>15.132293598692952</v>
+        <v>15.132293598692959</v>
       </c>
       <c r="K41" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I41,$H$5,$H$6)</f>
-        <v>15132.293598692951</v>
+        <v>15132.293598692959</v>
       </c>
       <c r="L41" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I41,$C$20,$H$5,$H$6)</f>
@@ -3853,7 +3859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:14" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:14" ht="24.9" x14ac:dyDescent="0.4">
       <c r="B42" s="17" t="s">
         <v>40</v>
       </c>
@@ -3871,11 +3877,11 @@
       </c>
       <c r="J42" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I42,$H$5,$H$6)/1000</f>
-        <v>15.132293890402293</v>
+        <v>15.1322938904023</v>
       </c>
       <c r="K42" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I42,$H$5,$H$6)</f>
-        <v>15132.293890402292</v>
+        <v>15132.293890402299</v>
       </c>
       <c r="L42" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I42,$C$20,$H$5,$H$6)</f>
@@ -3890,7 +3896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:14" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:14" ht="14.6" x14ac:dyDescent="0.4">
       <c r="B43" s="8"/>
       <c r="C43" s="13"/>
       <c r="D43" s="13"/>
@@ -3901,11 +3907,11 @@
       </c>
       <c r="J43" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I43,$H$5,$H$6)/1000</f>
-        <v>15.132293775802426</v>
+        <v>15.132293775802431</v>
       </c>
       <c r="K43" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I43,$H$5,$H$6)</f>
-        <v>15132.293775802425</v>
+        <v>15132.293775802431</v>
       </c>
       <c r="L43" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I43,$C$20,$H$5,$H$6)</f>
@@ -3920,7 +3926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:14" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:14" ht="14.6" x14ac:dyDescent="0.4">
       <c r="B44" s="8"/>
       <c r="C44" s="13"/>
       <c r="D44" s="13"/>
@@ -3931,11 +3937,11 @@
       </c>
       <c r="J44" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I44,$H$5,$H$6)/1000</f>
-        <v>15.13229377319759</v>
+        <v>15.132330117306124</v>
       </c>
       <c r="K44" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I44,$H$5,$H$6)</f>
-        <v>15132.293773197591</v>
+        <v>15132.330117306123</v>
       </c>
       <c r="L44" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I44,$C$20,$H$5,$H$6)</f>
@@ -3950,18 +3956,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:14" x14ac:dyDescent="0.3">
       <c r="I45" s="1">
         <f t="shared" si="2"/>
         <v>32.058823529411754</v>
       </c>
       <c r="J45" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I45,$H$5,$H$6)/1000</f>
-        <v>15.132293308285638</v>
+        <v>15.132339364156794</v>
       </c>
       <c r="K45" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I45,$H$5,$H$6)</f>
-        <v>15132.293308285638</v>
+        <v>15132.339364156793</v>
       </c>
       <c r="L45" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I45,$C$20,$H$5,$H$6)</f>
@@ -3976,18 +3982,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:14" x14ac:dyDescent="0.3">
       <c r="I46" s="1">
         <f t="shared" si="2"/>
         <v>33.470588235294109</v>
       </c>
       <c r="J46" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I46,$H$5,$H$6)/1000</f>
-        <v>15.132293396840248</v>
+        <v>15.132444305090065</v>
       </c>
       <c r="K46" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I46,$H$5,$H$6)</f>
-        <v>15132.293396840249</v>
+        <v>15132.444305090065</v>
       </c>
       <c r="L46" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I46,$C$20,$H$5,$H$6)</f>
@@ -4002,18 +4008,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:14" x14ac:dyDescent="0.3">
       <c r="I47" s="1">
         <f t="shared" si="2"/>
         <v>34.882352941176464</v>
       </c>
       <c r="J47" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I47,$H$5,$H$6)/1000</f>
-        <v>15.132293541392761</v>
+        <v>15.132593044874914</v>
       </c>
       <c r="K47" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I47,$H$5,$H$6)</f>
-        <v>15132.293541392761</v>
+        <v>15132.593044874915</v>
       </c>
       <c r="L47" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I47,$C$20,$H$5,$H$6)</f>
@@ -4028,18 +4034,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:14" x14ac:dyDescent="0.3">
       <c r="I48" s="1">
         <f t="shared" si="2"/>
         <v>36.294117647058819</v>
       </c>
       <c r="J48" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I48,$H$5,$H$6)/1000</f>
-        <v>15.132293252287734</v>
+        <v>15.132436227065908</v>
       </c>
       <c r="K48" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I48,$H$5,$H$6)</f>
-        <v>15132.293252287735</v>
+        <v>15132.436227065908</v>
       </c>
       <c r="L48" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I48,$C$20,$H$5,$H$6)</f>
@@ -4054,18 +4060,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="9:14" x14ac:dyDescent="0.35">
+    <row r="49" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I49" s="1">
         <f t="shared" si="2"/>
         <v>37.705882352941174</v>
       </c>
       <c r="J49" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I49,$H$5,$H$6)/1000</f>
-        <v>15.132293714595367</v>
+        <v>15.132317098549965</v>
       </c>
       <c r="K49" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I49,$H$5,$H$6)</f>
-        <v>15132.293714595367</v>
+        <v>15132.317098549966</v>
       </c>
       <c r="L49" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I49,$C$20,$H$5,$H$6)</f>
@@ -4080,18 +4086,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="9:14" x14ac:dyDescent="0.35">
+    <row r="50" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I50" s="1">
         <f t="shared" si="2"/>
         <v>39.117647058823529</v>
       </c>
       <c r="J50" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I50,$H$5,$H$6)/1000</f>
-        <v>15.132293916447811</v>
+        <v>15.132421149090058</v>
       </c>
       <c r="K50" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I50,$H$5,$H$6)</f>
-        <v>15132.29391644781</v>
+        <v>15132.421149090058</v>
       </c>
       <c r="L50" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I50,$C$20,$H$5,$H$6)</f>
@@ -4106,18 +4112,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="9:14" x14ac:dyDescent="0.35">
+    <row r="51" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I51" s="1">
         <f t="shared" si="2"/>
         <v>40.529411764705884</v>
       </c>
       <c r="J51" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I51,$H$5,$H$6)/1000</f>
-        <v>15.123567390728281</v>
+        <v>15.123567390728287</v>
       </c>
       <c r="K51" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I51,$H$5,$H$6)</f>
-        <v>15123.567390728282</v>
+        <v>15123.567390728287</v>
       </c>
       <c r="L51" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I51,$C$20,$H$5,$H$6)</f>
@@ -4132,18 +4138,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="9:14" x14ac:dyDescent="0.35">
+    <row r="52" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I52" s="1">
         <f t="shared" si="2"/>
         <v>41.941176470588239</v>
       </c>
       <c r="J52" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I52,$H$5,$H$6)/1000</f>
-        <v>15.087810103088721</v>
+        <v>15.087823257771033</v>
       </c>
       <c r="K52" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I52,$H$5,$H$6)</f>
-        <v>15087.810103088721</v>
+        <v>15087.823257771033</v>
       </c>
       <c r="L52" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I52,$C$20,$H$5,$H$6)</f>
@@ -4158,18 +4164,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="9:14" x14ac:dyDescent="0.35">
+    <row r="53" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I53" s="1">
         <f t="shared" si="2"/>
         <v>43.352941176470594</v>
       </c>
       <c r="J53" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I53,$H$5,$H$6)/1000</f>
-        <v>15.024040340821331</v>
+        <v>15.024088805923846</v>
       </c>
       <c r="K53" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I53,$H$5,$H$6)</f>
-        <v>15024.040340821331</v>
+        <v>15024.088805923846</v>
       </c>
       <c r="L53" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I53,$C$20,$H$5,$H$6)</f>
@@ -4184,18 +4190,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="9:14" x14ac:dyDescent="0.35">
+    <row r="54" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I54" s="1">
         <f t="shared" si="2"/>
         <v>44.764705882352949</v>
       </c>
       <c r="J54" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I54,$H$5,$H$6)/1000</f>
-        <v>14.931698783899501</v>
+        <v>14.931930165945385</v>
       </c>
       <c r="K54" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I54,$H$5,$H$6)</f>
-        <v>14931.698783899501</v>
+        <v>14931.930165945385</v>
       </c>
       <c r="L54" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I54,$C$20,$H$5,$H$6)</f>
@@ -4210,18 +4216,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="9:14" x14ac:dyDescent="0.35">
+    <row r="55" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I55" s="1">
         <f t="shared" si="2"/>
         <v>46.176470588235304</v>
       </c>
       <c r="J55" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I55,$H$5,$H$6)/1000</f>
-        <v>14.81007554969816</v>
+        <v>14.810117273269569</v>
       </c>
       <c r="K55" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I55,$H$5,$H$6)</f>
-        <v>14810.07554969816</v>
+        <v>14810.117273269569</v>
       </c>
       <c r="L55" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I55,$C$20,$H$5,$H$6)</f>
@@ -4236,18 +4242,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="9:14" x14ac:dyDescent="0.35">
+    <row r="56" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I56" s="1">
         <f t="shared" si="2"/>
         <v>47.588235294117659</v>
       </c>
       <c r="J56" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I56,$H$5,$H$6)/1000</f>
-        <v>14.658285117179609</v>
+        <v>14.658285117179615</v>
       </c>
       <c r="K56" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I56,$H$5,$H$6)</f>
-        <v>14658.28511717961</v>
+        <v>14658.285117179616</v>
       </c>
       <c r="L56" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I56,$C$20,$H$5,$H$6)</f>
@@ -4262,18 +4268,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="9:14" x14ac:dyDescent="0.35">
+    <row r="57" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I57" s="1">
         <f t="shared" si="2"/>
         <v>49.000000000000014</v>
       </c>
       <c r="J57" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I57,$H$5,$H$6)/1000</f>
-        <v>14.475242195036955</v>
+        <v>14.475242195036961</v>
       </c>
       <c r="K57" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I57,$H$5,$H$6)</f>
-        <v>14475.242195036955</v>
+        <v>14475.242195036961</v>
       </c>
       <c r="L57" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I57,$C$20,$H$5,$H$6)</f>
@@ -4288,22 +4294,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="9:14" x14ac:dyDescent="0.35">
+    <row r="58" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I58" s="1">
         <f t="shared" si="2"/>
         <v>50.411764705882369</v>
       </c>
       <c r="J58" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I58,$H$5,$H$6)/1000</f>
-        <v>14.259626207372431</v>
+        <v>14.259812715443463</v>
       </c>
       <c r="K58" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I58,$H$5,$H$6)</f>
-        <v>14259.626207372432</v>
+        <v>14259.812715443462</v>
       </c>
       <c r="L58" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I58,$C$20,$H$5,$H$6)</f>
-        <v>2010.4554333110036</v>
+        <v>2010.489179858429</v>
       </c>
       <c r="M58" s="1">
         <f t="shared" si="3"/>
@@ -4314,22 +4320,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="9:14" x14ac:dyDescent="0.35">
+    <row r="59" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I59" s="1">
         <f t="shared" si="2"/>
         <v>51.823529411764724</v>
       </c>
       <c r="J59" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I59,$H$5,$H$6)/1000</f>
-        <v>14.009829781204479</v>
+        <v>14.009855395414645</v>
       </c>
       <c r="K59" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I59,$H$5,$H$6)</f>
-        <v>14009.829781204478</v>
+        <v>14009.855395414645</v>
       </c>
       <c r="L59" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I59,$C$20,$H$5,$H$6)</f>
-        <v>4224.127282929594</v>
+        <v>4224.1429980100538</v>
       </c>
       <c r="M59" s="1">
         <f t="shared" si="3"/>
@@ -4340,22 +4346,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="9:14" x14ac:dyDescent="0.35">
+    <row r="60" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I60" s="1">
         <f t="shared" si="2"/>
         <v>53.235294117647079</v>
       </c>
       <c r="J60" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I60,$H$5,$H$6)/1000</f>
-        <v>13.723900434714098</v>
+        <v>13.723985036855227</v>
       </c>
       <c r="K60" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I60,$H$5,$H$6)</f>
-        <v>13723.900434714098</v>
+        <v>13723.985036855227</v>
       </c>
       <c r="L60" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I60,$C$20,$H$5,$H$6)</f>
-        <v>5617.4531638038306</v>
+        <v>5617.5065273126429</v>
       </c>
       <c r="M60" s="1">
         <f t="shared" si="3"/>
@@ -4366,22 +4372,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="9:14" x14ac:dyDescent="0.35">
+    <row r="61" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I61" s="1">
         <f t="shared" si="2"/>
         <v>54.647058823529434</v>
       </c>
       <c r="J61" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I61,$H$5,$H$6)/1000</f>
-        <v>13.399451233769602</v>
+        <v>13.399611072142129</v>
       </c>
       <c r="K61" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I61,$H$5,$H$6)</f>
-        <v>13399.451233769601</v>
+        <v>13399.611072142128</v>
       </c>
       <c r="L61" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I61,$C$20,$H$5,$H$6)</f>
-        <v>6721.4968695038351</v>
+        <v>6721.5078792603445</v>
       </c>
       <c r="M61" s="1">
         <f t="shared" si="3"/>
@@ -4392,22 +4398,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="9:14" x14ac:dyDescent="0.35">
+    <row r="62" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I62" s="1">
         <f t="shared" si="2"/>
         <v>56.058823529411789</v>
       </c>
       <c r="J62" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I62,$H$5,$H$6)/1000</f>
-        <v>13.033546109785838</v>
+        <v>13.033611809348725</v>
       </c>
       <c r="K62" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I62,$H$5,$H$6)</f>
-        <v>13033.546109785839</v>
+        <v>13033.611809348726</v>
       </c>
       <c r="L62" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I62,$C$20,$H$5,$H$6)</f>
-        <v>7662.2948100973299</v>
+        <v>7662.4475042268123</v>
       </c>
       <c r="M62" s="1">
         <f t="shared" si="3"/>
@@ -4418,22 +4424,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="9:14" x14ac:dyDescent="0.35">
+    <row r="63" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I63" s="1">
         <f t="shared" si="2"/>
         <v>57.470588235294144</v>
       </c>
       <c r="J63" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I63,$H$5,$H$6)/1000</f>
-        <v>12.62253106481289</v>
+        <v>12.622558699543063</v>
       </c>
       <c r="K63" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I63,$H$5,$H$6)</f>
-        <v>12622.531064812889</v>
+        <v>12622.558699543064</v>
       </c>
       <c r="L63" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I63,$C$20,$H$5,$H$6)</f>
-        <v>8494.2367807027476</v>
+        <v>8494.2695361293008</v>
       </c>
       <c r="M63" s="1">
         <f t="shared" si="3"/>
@@ -4444,22 +4450,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="9:14" x14ac:dyDescent="0.35">
+    <row r="64" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I64" s="1">
         <f t="shared" si="2"/>
         <v>58.882352941176499</v>
       </c>
       <c r="J64" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I64,$H$5,$H$6)/1000</f>
-        <v>12.16179712257922</v>
+        <v>12.161862989000682</v>
       </c>
       <c r="K64" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I64,$H$5,$H$6)</f>
-        <v>12161.797122579219</v>
+        <v>12161.862989000681</v>
       </c>
       <c r="L64" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I64,$C$20,$H$5,$H$6)</f>
-        <v>9246.7388977730516</v>
+        <v>9246.8116227220344</v>
       </c>
       <c r="M64" s="1">
         <f t="shared" si="3"/>
@@ -4470,22 +4476,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="9:14" x14ac:dyDescent="0.35">
+    <row r="65" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I65" s="1">
         <f t="shared" si="2"/>
         <v>60.294117647058854</v>
       </c>
       <c r="J65" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I65,$H$5,$H$6)/1000</f>
-        <v>11.645419699120408</v>
+        <v>11.645470475847967</v>
       </c>
       <c r="K65" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I65,$H$5,$H$6)</f>
-        <v>11645.419699120408</v>
+        <v>11645.470475847967</v>
       </c>
       <c r="L65" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I65,$C$20,$H$5,$H$6)</f>
-        <v>9937.8601081679808</v>
+        <v>9937.9309340547898</v>
       </c>
       <c r="M65" s="1">
         <f t="shared" si="3"/>
@@ -4496,22 +4502,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="9:14" x14ac:dyDescent="0.35">
+    <row r="66" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I66" s="1">
         <f t="shared" si="2"/>
         <v>61.705882352941209</v>
       </c>
       <c r="J66" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I66,$H$5,$H$6)/1000</f>
-        <v>11.065595095987858</v>
+        <v>11.065613139281119</v>
       </c>
       <c r="K66" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I66,$H$5,$H$6)</f>
-        <v>11065.595095987857</v>
+        <v>11065.613139281118</v>
       </c>
       <c r="L66" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I66,$C$20,$H$5,$H$6)</f>
-        <v>10579.643235636535</v>
+        <v>10579.655322593395</v>
       </c>
       <c r="M66" s="1">
         <f t="shared" si="3"/>
@@ -4522,22 +4528,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="9:14" x14ac:dyDescent="0.35">
+    <row r="67" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I67" s="1">
         <f t="shared" si="2"/>
         <v>63.117647058823565</v>
       </c>
       <c r="J67" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I67,$H$5,$H$6)/1000</f>
-        <v>10.411724986497131</v>
+        <v>10.411738924275026</v>
       </c>
       <c r="K67" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I67,$H$5,$H$6)</f>
-        <v>10411.724986497131</v>
+        <v>10411.738924275027</v>
       </c>
       <c r="L67" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I67,$C$20,$H$5,$H$6)</f>
-        <v>11180.600817008482</v>
+        <v>11180.613996804726</v>
       </c>
       <c r="M67" s="1">
         <f t="shared" si="3"/>
@@ -4548,22 +4554,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="9:14" x14ac:dyDescent="0.35">
+    <row r="68" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I68" s="1">
         <f t="shared" si="2"/>
         <v>64.529411764705912</v>
       </c>
       <c r="J68" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I68,$H$5,$H$6)/1000</f>
-        <v>9.6688049835757255</v>
+        <v>9.6688968073502775</v>
       </c>
       <c r="K68" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I68,$H$5,$H$6)</f>
-        <v>9668.8049835757247</v>
+        <v>9668.8968073502783</v>
       </c>
       <c r="L68" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I68,$C$20,$H$5,$H$6)</f>
-        <v>11747.01748739508</v>
+        <v>11747.101303961043</v>
       </c>
       <c r="M68" s="1">
         <f t="shared" si="3"/>
@@ -4574,22 +4580,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="9:14" x14ac:dyDescent="0.35">
+    <row r="69" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I69" s="1">
         <f t="shared" si="2"/>
         <v>65.94117647058826</v>
       </c>
       <c r="J69" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I69,$H$5,$H$6)/1000</f>
-        <v>8.8143645636878318</v>
+        <v>8.8144424417758298</v>
       </c>
       <c r="K69" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I69,$H$5,$H$6)</f>
-        <v>8814.3645636878318</v>
+        <v>8814.4424417758291</v>
       </c>
       <c r="L69" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I69,$C$20,$H$5,$H$6)</f>
-        <v>12283.694167692429</v>
+        <v>12283.694167692433</v>
       </c>
       <c r="M69" s="1">
         <f t="shared" si="3"/>
@@ -4600,22 +4606,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="9:14" x14ac:dyDescent="0.35">
+    <row r="70" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I70" s="1">
         <f t="shared" si="2"/>
         <v>67.352941176470608</v>
       </c>
       <c r="J70" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I70,$H$5,$H$6)/1000</f>
-        <v>7.8119276946842753</v>
+        <v>7.8119570849652993</v>
       </c>
       <c r="K70" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I70,$H$5,$H$6)</f>
-        <v>7811.9276946842756</v>
+        <v>7811.9570849652991</v>
       </c>
       <c r="L70" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I70,$C$20,$H$5,$H$6)</f>
-        <v>12794.396624196695</v>
+        <v>12794.551782045031</v>
       </c>
       <c r="M70" s="1">
         <f t="shared" si="3"/>
@@ -4623,25 +4629,25 @@
       </c>
       <c r="N70" s="1">
         <f t="shared" si="4"/>
-        <v>12794.396624196695</v>
-      </c>
-    </row>
-    <row r="71" spans="9:14" x14ac:dyDescent="0.35">
+        <v>12794.551782045031</v>
+      </c>
+    </row>
+    <row r="71" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I71" s="1">
         <f t="shared" si="2"/>
         <v>68.764705882352956</v>
       </c>
       <c r="J71" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I71,$H$5,$H$6)/1000</f>
-        <v>6.5943921634374583</v>
+        <v>6.5943921634374618</v>
       </c>
       <c r="K71" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I71,$H$5,$H$6)</f>
-        <v>6594.3921634374583</v>
+        <v>6594.3921634374619</v>
       </c>
       <c r="L71" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I71,$C$20,$H$5,$H$6)</f>
-        <v>13282.150153055929</v>
+        <v>13282.335488606182</v>
       </c>
       <c r="M71" s="1">
         <f t="shared" si="3"/>
@@ -4649,25 +4655,25 @@
       </c>
       <c r="N71" s="1">
         <f t="shared" si="4"/>
-        <v>13282.150153055929</v>
-      </c>
-    </row>
-    <row r="72" spans="9:14" x14ac:dyDescent="0.35">
+        <v>13282.335488606182</v>
+      </c>
+    </row>
+    <row r="72" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I72" s="1">
         <f t="shared" si="2"/>
         <v>70.176470588235304</v>
       </c>
       <c r="J72" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I72,$H$5,$H$6)/1000</f>
-        <v>5.0073142166949998</v>
+        <v>5.0073796364780643</v>
       </c>
       <c r="K72" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I72,$H$5,$H$6)</f>
-        <v>5007.3142166950001</v>
+        <v>5007.3796364780646</v>
       </c>
       <c r="L72" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I72,$C$20,$H$5,$H$6)</f>
-        <v>13749.423910087005</v>
+        <v>13749.522711983491</v>
       </c>
       <c r="M72" s="1">
         <f t="shared" si="3"/>
@@ -4675,25 +4681,25 @@
       </c>
       <c r="N72" s="1">
         <f t="shared" si="4"/>
-        <v>13749.423910087005</v>
-      </c>
-    </row>
-    <row r="73" spans="9:14" x14ac:dyDescent="0.35">
+        <v>13749.522711983491</v>
+      </c>
+    </row>
+    <row r="73" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I73" s="1">
         <f t="shared" si="2"/>
         <v>71.588235294117652</v>
       </c>
       <c r="J73" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I73,$H$5,$H$6)/1000</f>
-        <v>2.4059714599975983</v>
+        <v>2.4060122810436479</v>
       </c>
       <c r="K73" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I73,$H$5,$H$6)</f>
-        <v>2405.9714599975982</v>
+        <v>2406.0122810436478</v>
       </c>
       <c r="L73" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I73,$C$20,$H$5,$H$6)</f>
-        <v>14198.269666518319</v>
+        <v>14198.306787296195</v>
       </c>
       <c r="M73" s="1">
         <f t="shared" si="3"/>
@@ -4701,10 +4707,10 @@
       </c>
       <c r="N73" s="1">
         <f t="shared" si="4"/>
-        <v>14198.269666518319</v>
-      </c>
-    </row>
-    <row r="74" spans="9:14" x14ac:dyDescent="0.35">
+        <v>14198.306787296195</v>
+      </c>
+    </row>
+    <row r="74" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I74" s="1">
         <f t="shared" si="2"/>
         <v>73</v>
@@ -4719,18 +4725,18 @@
       </c>
       <c r="L74" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I74,$C$20,$H$5,$H$6)</f>
-        <v>14630.414688406485</v>
+        <v>14630.446737999669</v>
       </c>
       <c r="M74" s="1">
         <f t="shared" si="3"/>
-        <v>14630.414688406485</v>
+        <v>14630.446737999669</v>
       </c>
       <c r="N74" s="1">
         <f t="shared" si="4"/>
-        <v>14630.414688406485</v>
-      </c>
-    </row>
-    <row r="75" spans="9:14" x14ac:dyDescent="0.35">
+        <v>14630.446737999669</v>
+      </c>
+    </row>
+    <row r="75" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I75" s="1">
         <f t="shared" si="2"/>
         <v>74.411764705882348</v>
@@ -4745,18 +4751,18 @@
       </c>
       <c r="L75" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I75,$C$20,$H$5,$H$6)</f>
-        <v>15047.328305168016</v>
+        <v>15047.369694955658</v>
       </c>
       <c r="M75" s="1">
         <f t="shared" si="3"/>
-        <v>15047.328305168016</v>
+        <v>15047.369694955658</v>
       </c>
       <c r="N75" s="1">
         <f t="shared" si="4"/>
-        <v>15047.328305168016</v>
-      </c>
-    </row>
-    <row r="76" spans="9:14" x14ac:dyDescent="0.35">
+        <v>15047.369694955658</v>
+      </c>
+    </row>
+    <row r="76" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I76" s="1">
         <f t="shared" si="2"/>
         <v>75.823529411764696</v>
@@ -4771,18 +4777,18 @@
       </c>
       <c r="L76" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I76,$C$20,$H$5,$H$6)</f>
-        <v>15450.274923663121</v>
+        <v>15450.274923663128</v>
       </c>
       <c r="M76" s="1">
         <f t="shared" si="3"/>
-        <v>15450.274923663121</v>
+        <v>15450.274923663128</v>
       </c>
       <c r="N76" s="1">
         <f t="shared" si="4"/>
-        <v>15450.274923663121</v>
-      </c>
-    </row>
-    <row r="77" spans="9:14" x14ac:dyDescent="0.35">
+        <v>15450.274923663128</v>
+      </c>
+    </row>
+    <row r="77" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I77" s="1">
         <f t="shared" si="2"/>
         <v>77.235294117647044</v>
@@ -4797,18 +4803,18 @@
       </c>
       <c r="L77" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I77,$C$20,$H$5,$H$6)</f>
-        <v>15840.351571150621</v>
+        <v>15844.147396689053</v>
       </c>
       <c r="M77" s="1">
         <f t="shared" si="3"/>
-        <v>15840.351571150621</v>
+        <v>15844.147396689053</v>
       </c>
       <c r="N77" s="1">
         <f t="shared" si="4"/>
-        <v>15840.351571150621</v>
-      </c>
-    </row>
-    <row r="78" spans="9:14" x14ac:dyDescent="0.35">
+        <v>15844.147396689053</v>
+      </c>
+    </row>
+    <row r="78" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I78" s="1">
         <f t="shared" si="2"/>
         <v>78.647058823529392</v>
@@ -4823,18 +4829,18 @@
       </c>
       <c r="L78" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I78,$C$20,$H$5,$H$6)</f>
-        <v>16218.518742724227</v>
+        <v>16218.518742724234</v>
       </c>
       <c r="M78" s="1">
         <f t="shared" si="3"/>
-        <v>16218.518742724227</v>
+        <v>16218.518742724234</v>
       </c>
       <c r="N78" s="1">
         <f t="shared" si="4"/>
-        <v>16218.518742724227</v>
-      </c>
-    </row>
-    <row r="79" spans="9:14" x14ac:dyDescent="0.35">
+        <v>16218.518742724234</v>
+      </c>
+    </row>
+    <row r="79" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I79" s="1">
         <f t="shared" si="2"/>
         <v>80.05882352941174</v>
@@ -4849,18 +4855,18 @@
       </c>
       <c r="L79" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I79,$C$20,$H$5,$H$6)</f>
-        <v>16585.622292462373</v>
+        <v>16585.680858167587</v>
       </c>
       <c r="M79" s="1">
         <f t="shared" si="3"/>
-        <v>16585.622292462373</v>
+        <v>16585.680858167587</v>
       </c>
       <c r="N79" s="1">
         <f t="shared" si="4"/>
-        <v>16585.622292462373</v>
-      </c>
-    </row>
-    <row r="80" spans="9:14" x14ac:dyDescent="0.35">
+        <v>16585.680858167587</v>
+      </c>
+    </row>
+    <row r="80" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I80" s="1">
         <f t="shared" si="2"/>
         <v>81.470588235294088</v>
@@ -4875,18 +4881,18 @@
       </c>
       <c r="L80" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I80,$C$20,$H$5,$H$6)</f>
-        <v>16942.411442652079</v>
+        <v>16942.411442652083</v>
       </c>
       <c r="M80" s="1">
         <f t="shared" si="3"/>
-        <v>16942.411442652079</v>
+        <v>16942.411442652083</v>
       </c>
       <c r="N80" s="1">
         <f t="shared" si="4"/>
-        <v>16942.411442652079</v>
-      </c>
-    </row>
-    <row r="81" spans="9:14" x14ac:dyDescent="0.35">
+        <v>16942.411442652083</v>
+      </c>
+    </row>
+    <row r="81" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I81" s="1">
         <f t="shared" si="2"/>
         <v>82.882352941176435</v>
@@ -4901,18 +4907,18 @@
       </c>
       <c r="L81" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I81,$C$20,$H$5,$H$6)</f>
-        <v>17289.55520135515</v>
+        <v>17289.614197050938</v>
       </c>
       <c r="M81" s="1">
         <f t="shared" si="3"/>
-        <v>17289.55520135515</v>
+        <v>17289.614197050938</v>
       </c>
       <c r="N81" s="1">
         <f t="shared" si="4"/>
-        <v>17289.55520135515</v>
-      </c>
-    </row>
-    <row r="82" spans="9:14" x14ac:dyDescent="0.35">
+        <v>17289.614197050938</v>
+      </c>
+    </row>
+    <row r="82" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I82" s="1">
         <f t="shared" si="2"/>
         <v>84.294117647058783</v>
@@ -4927,18 +4933,18 @@
       </c>
       <c r="L82" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I82,$C$20,$H$5,$H$6)</f>
-        <v>17627.654061073394</v>
+        <v>17627.680677787979</v>
       </c>
       <c r="M82" s="1">
         <f t="shared" si="3"/>
-        <v>17627.654061073394</v>
+        <v>17627.680677787979</v>
       </c>
       <c r="N82" s="1">
         <f t="shared" si="4"/>
-        <v>17627.654061073394</v>
-      </c>
-    </row>
-    <row r="83" spans="9:14" x14ac:dyDescent="0.35">
+        <v>17627.680677787979</v>
+      </c>
+    </row>
+    <row r="83" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I83" s="1">
         <f t="shared" si="2"/>
         <v>85.705882352941131</v>
@@ -4953,18 +4959,18 @@
       </c>
       <c r="L83" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I83,$C$20,$H$5,$H$6)</f>
-        <v>17957.247774838354</v>
+        <v>17957.346134896223</v>
       </c>
       <c r="M83" s="1">
         <f t="shared" si="3"/>
-        <v>17957.247774838354</v>
+        <v>17957.346134896223</v>
       </c>
       <c r="N83" s="1">
         <f t="shared" si="4"/>
-        <v>17957.247774838354</v>
-      </c>
-    </row>
-    <row r="84" spans="9:14" x14ac:dyDescent="0.35">
+        <v>17957.346134896223</v>
+      </c>
+    </row>
+    <row r="84" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I84" s="1">
         <f t="shared" si="2"/>
         <v>87.117647058823479</v>
@@ -4979,18 +4985,18 @@
       </c>
       <c r="L84" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I84,$C$20,$H$5,$H$6)</f>
-        <v>18278.825823409399</v>
+        <v>18278.854772828065</v>
       </c>
       <c r="M84" s="1">
         <f t="shared" si="3"/>
-        <v>18278.825823409399</v>
+        <v>18278.854772828065</v>
       </c>
       <c r="N84" s="1">
         <f t="shared" si="4"/>
-        <v>18278.825823409399</v>
-      </c>
-    </row>
-    <row r="85" spans="9:14" x14ac:dyDescent="0.35">
+        <v>18278.854772828065</v>
+      </c>
+    </row>
+    <row r="85" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I85" s="1">
         <f t="shared" si="2"/>
         <v>88.529411764705827</v>
@@ -5005,18 +5011,18 @@
       </c>
       <c r="L85" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I85,$C$20,$H$5,$H$6)</f>
-        <v>18592.83192811739</v>
+        <v>18593.504749915024</v>
       </c>
       <c r="M85" s="1">
         <f t="shared" si="3"/>
-        <v>18592.83192811739</v>
+        <v>18593.504749915024</v>
       </c>
       <c r="N85" s="1">
         <f t="shared" si="4"/>
-        <v>18592.83192811739</v>
-      </c>
-    </row>
-    <row r="86" spans="9:14" x14ac:dyDescent="0.35">
+        <v>18593.504749915024</v>
+      </c>
+    </row>
+    <row r="86" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I86" s="1">
         <f t="shared" si="2"/>
         <v>89.941176470588175</v>
@@ -5031,18 +5037,18 @@
       </c>
       <c r="L86" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I86,$C$20,$H$5,$H$6)</f>
-        <v>18899.671325158339</v>
+        <v>18899.6877139922</v>
       </c>
       <c r="M86" s="1">
         <f t="shared" si="3"/>
-        <v>18899.671325158339</v>
+        <v>18899.6877139922</v>
       </c>
       <c r="N86" s="1">
         <f t="shared" si="4"/>
-        <v>18899.671325158339</v>
-      </c>
-    </row>
-    <row r="87" spans="9:14" x14ac:dyDescent="0.35">
+        <v>18899.6877139922</v>
+      </c>
+    </row>
+    <row r="87" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I87" s="1">
         <f t="shared" si="2"/>
         <v>91.352941176470523</v>
@@ -5057,18 +5063,18 @@
       </c>
       <c r="L87" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I87,$C$20,$H$5,$H$6)</f>
-        <v>19199.715657092231</v>
+        <v>19199.901980928051</v>
       </c>
       <c r="M87" s="1">
         <f t="shared" ref="M87:M99" si="5">IF(I87&gt;$C$40,L87,0)</f>
-        <v>19199.715657092231</v>
+        <v>19199.901980928051</v>
       </c>
       <c r="N87" s="1">
         <f t="shared" ref="N87:N99" si="6">IF(I87&gt;$C$39,L87,0)</f>
-        <v>19199.715657092231</v>
-      </c>
-    </row>
-    <row r="88" spans="9:14" x14ac:dyDescent="0.35">
+        <v>19199.901980928051</v>
+      </c>
+    </row>
+    <row r="88" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I88" s="1">
         <f t="shared" si="2"/>
         <v>92.764705882352871</v>
@@ -5083,18 +5089,18 @@
       </c>
       <c r="L88" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I88,$C$20,$H$5,$H$6)</f>
-        <v>19496.426925926004</v>
+        <v>19496.48142348669</v>
       </c>
       <c r="M88" s="1">
         <f t="shared" si="5"/>
-        <v>19496.426925926004</v>
+        <v>19496.48142348669</v>
       </c>
       <c r="N88" s="1">
         <f t="shared" si="6"/>
-        <v>19496.426925926004</v>
-      </c>
-    </row>
-    <row r="89" spans="9:14" x14ac:dyDescent="0.35">
+        <v>19496.48142348669</v>
+      </c>
+    </row>
+    <row r="89" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I89" s="1">
         <f t="shared" ref="I89:I99" si="7">I88+$I$21/51</f>
         <v>94.176470588235219</v>
@@ -5109,18 +5115,18 @@
       </c>
       <c r="L89" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I89,$C$20,$H$5,$H$6)</f>
-        <v>19793.138845896636</v>
+        <v>19793.154075247352</v>
       </c>
       <c r="M89" s="1">
         <f t="shared" si="5"/>
-        <v>19793.138845896636</v>
+        <v>19793.154075247352</v>
       </c>
       <c r="N89" s="1">
         <f t="shared" si="6"/>
-        <v>19793.138845896636</v>
-      </c>
-    </row>
-    <row r="90" spans="9:14" x14ac:dyDescent="0.35">
+        <v>19793.154075247352</v>
+      </c>
+    </row>
+    <row r="90" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I90" s="1">
         <f t="shared" si="7"/>
         <v>95.588235294117567</v>
@@ -5135,18 +5141,18 @@
       </c>
       <c r="L90" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I90,$C$20,$H$5,$H$6)</f>
-        <v>20089.850497598603</v>
+        <v>20089.929004556132</v>
       </c>
       <c r="M90" s="1">
         <f t="shared" si="5"/>
-        <v>20089.850497598603</v>
+        <v>20089.929004556132</v>
       </c>
       <c r="N90" s="1">
         <f t="shared" si="6"/>
-        <v>20089.850497598603</v>
-      </c>
-    </row>
-    <row r="91" spans="9:14" x14ac:dyDescent="0.35">
+        <v>20089.929004556132</v>
+      </c>
+    </row>
+    <row r="91" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I91" s="1">
         <f t="shared" si="7"/>
         <v>96.999999999999915</v>
@@ -5161,18 +5167,18 @@
       </c>
       <c r="L91" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I91,$C$20,$H$5,$H$6)</f>
-        <v>20386.562100465428</v>
+        <v>20386.596363812845</v>
       </c>
       <c r="M91" s="1">
         <f t="shared" si="5"/>
-        <v>20386.562100465428</v>
+        <v>20386.596363812845</v>
       </c>
       <c r="N91" s="1">
         <f t="shared" si="6"/>
-        <v>20386.562100465428</v>
-      </c>
-    </row>
-    <row r="92" spans="9:14" x14ac:dyDescent="0.35">
+        <v>20386.596363812845</v>
+      </c>
+    </row>
+    <row r="92" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I92" s="1">
         <f t="shared" si="7"/>
         <v>98.411764705882263</v>
@@ -5187,18 +5193,18 @@
       </c>
       <c r="L92" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I92,$C$20,$H$5,$H$6)</f>
-        <v>20683.273903882506</v>
+        <v>20683.372066720633</v>
       </c>
       <c r="M92" s="1">
         <f t="shared" si="5"/>
-        <v>20683.273903882506</v>
+        <v>20683.372066720633</v>
       </c>
       <c r="N92" s="1">
         <f t="shared" si="6"/>
-        <v>20683.273903882506</v>
-      </c>
-    </row>
-    <row r="93" spans="9:14" x14ac:dyDescent="0.35">
+        <v>20683.372066720633</v>
+      </c>
+    </row>
+    <row r="93" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I93" s="1">
         <f t="shared" si="7"/>
         <v>99.823529411764611</v>
@@ -5213,18 +5219,18 @@
       </c>
       <c r="L93" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I93,$C$20,$H$5,$H$6)</f>
-        <v>20979.985094579846</v>
+        <v>20980.03300848461</v>
       </c>
       <c r="M93" s="1">
         <f t="shared" si="5"/>
-        <v>20979.985094579846</v>
+        <v>20980.03300848461</v>
       </c>
       <c r="N93" s="1">
         <f t="shared" si="6"/>
-        <v>20979.985094579846</v>
-      </c>
-    </row>
-    <row r="94" spans="9:14" x14ac:dyDescent="0.35">
+        <v>20980.03300848461</v>
+      </c>
+    </row>
+    <row r="94" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I94" s="1">
         <f t="shared" si="7"/>
         <v>101.23529411764696</v>
@@ -5239,18 +5245,18 @@
       </c>
       <c r="L94" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I94,$C$20,$H$5,$H$6)</f>
-        <v>21276.697456021215</v>
+        <v>21276.766733582681</v>
       </c>
       <c r="M94" s="1">
         <f t="shared" si="5"/>
-        <v>21276.697456021215</v>
+        <v>21276.766733582681</v>
       </c>
       <c r="N94" s="1">
         <f t="shared" si="6"/>
-        <v>21276.697456021215</v>
-      </c>
-    </row>
-    <row r="95" spans="9:14" x14ac:dyDescent="0.35">
+        <v>21276.766733582681</v>
+      </c>
+    </row>
+    <row r="95" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I95" s="1">
         <f t="shared" si="7"/>
         <v>102.64705882352931</v>
@@ -5265,18 +5271,18 @@
       </c>
       <c r="L95" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I95,$C$20,$H$5,$H$6)</f>
-        <v>21573.408411006203</v>
+        <v>21573.469266751661</v>
       </c>
       <c r="M95" s="1">
         <f t="shared" si="5"/>
-        <v>21573.408411006203</v>
+        <v>21573.469266751661</v>
       </c>
       <c r="N95" s="1">
         <f t="shared" si="6"/>
-        <v>21573.408411006203</v>
-      </c>
-    </row>
-    <row r="96" spans="9:14" x14ac:dyDescent="0.35">
+        <v>21573.469266751661</v>
+      </c>
+    </row>
+    <row r="96" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I96" s="1">
         <f t="shared" si="7"/>
         <v>104.05882352941165</v>
@@ -5291,18 +5297,18 @@
       </c>
       <c r="L96" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I96,$C$20,$H$5,$H$6)</f>
-        <v>21870.119931178731</v>
+        <v>21870.245663779282</v>
       </c>
       <c r="M96" s="1">
         <f t="shared" si="5"/>
-        <v>21870.119931178731</v>
+        <v>21870.245663779282</v>
       </c>
       <c r="N96" s="1">
         <f t="shared" si="6"/>
-        <v>21870.119931178731</v>
-      </c>
-    </row>
-    <row r="97" spans="9:14" x14ac:dyDescent="0.35">
+        <v>21870.245663779282</v>
+      </c>
+    </row>
+    <row r="97" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I97" s="1">
         <f t="shared" si="7"/>
         <v>105.470588235294</v>
@@ -5317,18 +5323,18 @@
       </c>
       <c r="L97" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I97,$C$20,$H$5,$H$6)</f>
-        <v>22166.831814685807</v>
+        <v>22166.875820776397</v>
       </c>
       <c r="M97" s="1">
         <f t="shared" si="5"/>
-        <v>22166.831814685807</v>
+        <v>22166.875820776397</v>
       </c>
       <c r="N97" s="1">
         <f t="shared" si="6"/>
-        <v>22166.831814685807</v>
-      </c>
-    </row>
-    <row r="98" spans="9:14" x14ac:dyDescent="0.35">
+        <v>22166.875820776397</v>
+      </c>
+    </row>
+    <row r="98" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I98" s="1">
         <f t="shared" si="7"/>
         <v>106.88235294117635</v>
@@ -5343,18 +5349,18 @@
       </c>
       <c r="L98" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I98,$C$20,$H$5,$H$6)</f>
-        <v>22463.543672147567</v>
+        <v>22463.773442080615</v>
       </c>
       <c r="M98" s="1">
         <f t="shared" si="5"/>
-        <v>22463.543672147567</v>
+        <v>22463.773442080615</v>
       </c>
       <c r="N98" s="1">
         <f t="shared" si="6"/>
-        <v>22463.543672147567</v>
-      </c>
-    </row>
-    <row r="99" spans="9:14" x14ac:dyDescent="0.35">
+        <v>22463.773442080615</v>
+      </c>
+    </row>
+    <row r="99" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I99" s="1">
         <f t="shared" si="7"/>
         <v>108.2941176470587</v>
@@ -5369,19 +5375,24 @@
       </c>
       <c r="L99" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I99,$C$20,$H$5,$H$6)</f>
-        <v>22760.255329709704</v>
+        <v>22760.290125397136</v>
       </c>
       <c r="M99" s="1">
         <f t="shared" si="5"/>
-        <v>22760.255329709704</v>
+        <v>22760.290125397136</v>
       </c>
       <c r="N99" s="1">
         <f t="shared" si="6"/>
-        <v>22760.255329709704</v>
+        <v>22760.290125397136</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C11:D11"/>
@@ -5389,11 +5400,6 @@
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
   </mergeCells>
   <conditionalFormatting sqref="C5:D5">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="lessThanOrEqual">

</xml_diff>

<commit_message>
ribbon update plus. bug with qliq in mf_pipe_atma fixed
</commit_message>
<xml_diff>
--- a/examples/ex120.GLV.xlsx
+++ b/examples/ex120.GLV.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <workbookPr codeName="ЭтаКнига" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\unifloc\unifloc_vba\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9BF1AED-7D89-4E53-A6C4-24099CA4DC29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A513F58-5A69-4AB4-A5F8-00C8282D74F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{7F603498-48FA-40A8-AB9B-D5E4C9CE020B}"/>
   </bookViews>
@@ -473,7 +473,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -539,30 +539,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="3" borderId="9" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -588,6 +564,31 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="9" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -683,7 +684,7 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>49.952452966948883</c:v>
+                  <c:v>49.873546067686959</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -695,7 +696,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>14326.055531312555</c:v>
+                  <c:v>16570.563391623593</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -717,160 +718,160 @@
             <c:numRef>
               <c:f>Клапана!$I$23:$I$73</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="51"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.4117647058823533</c:v>
+                  <c:v>2.5686274509803919</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.8235294117647065</c:v>
+                  <c:v>4.1372549019607838</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.2352941176470598</c:v>
+                  <c:v>5.7058823529411757</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.647058823529413</c:v>
+                  <c:v>7.2745098039215677</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.0588235294117663</c:v>
+                  <c:v>8.8431372549019596</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.4705882352941195</c:v>
+                  <c:v>10.411764705882351</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10.882352941176473</c:v>
+                  <c:v>11.980392156862743</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12.294117647058826</c:v>
+                  <c:v>13.549019607843135</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>13.705882352941179</c:v>
+                  <c:v>15.117647058823527</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>15.117647058823533</c:v>
+                  <c:v>16.686274509803919</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>16.529411764705884</c:v>
+                  <c:v>18.254901960784313</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>17.941176470588236</c:v>
+                  <c:v>19.823529411764707</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>19.352941176470587</c:v>
+                  <c:v>21.3921568627451</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>20.764705882352938</c:v>
+                  <c:v>22.960784313725494</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>22.17647058823529</c:v>
+                  <c:v>24.529411764705888</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>23.588235294117641</c:v>
+                  <c:v>26.098039215686281</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>24.999999999999993</c:v>
+                  <c:v>27.666666666666675</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>26.411764705882344</c:v>
+                  <c:v>29.235294117647069</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>27.823529411764696</c:v>
+                  <c:v>30.803921568627462</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>29.235294117647047</c:v>
+                  <c:v>32.372549019607852</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>30.647058823529399</c:v>
+                  <c:v>33.941176470588246</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>32.058823529411754</c:v>
+                  <c:v>35.50980392156864</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>33.470588235294109</c:v>
+                  <c:v>37.078431372549034</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>34.882352941176464</c:v>
+                  <c:v>38.647058823529427</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>36.294117647058819</c:v>
+                  <c:v>40.215686274509821</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>37.705882352941174</c:v>
+                  <c:v>41.784313725490215</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>39.117647058823529</c:v>
+                  <c:v>43.352941176470608</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>40.529411764705884</c:v>
+                  <c:v>44.921568627451002</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>41.941176470588239</c:v>
+                  <c:v>46.490196078431396</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>43.352941176470594</c:v>
+                  <c:v>48.058823529411789</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>44.764705882352949</c:v>
+                  <c:v>49.627450980392183</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>46.176470588235304</c:v>
+                  <c:v>51.196078431372577</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>47.588235294117659</c:v>
+                  <c:v>52.76470588235297</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>49.000000000000014</c:v>
+                  <c:v>54.333333333333364</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>50.411764705882369</c:v>
+                  <c:v>55.901960784313758</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>51.823529411764724</c:v>
+                  <c:v>57.470588235294152</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>53.235294117647079</c:v>
+                  <c:v>59.039215686274545</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>54.647058823529434</c:v>
+                  <c:v>60.607843137254939</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>56.058823529411789</c:v>
+                  <c:v>62.176470588235333</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>57.470588235294144</c:v>
+                  <c:v>63.745098039215726</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>58.882352941176499</c:v>
+                  <c:v>65.31372549019612</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>60.294117647058854</c:v>
+                  <c:v>66.882352941176507</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>61.705882352941209</c:v>
+                  <c:v>68.450980392156893</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>63.117647058823565</c:v>
+                  <c:v>70.01960784313728</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>64.529411764705912</c:v>
+                  <c:v>71.588235294117666</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>65.94117647058826</c:v>
+                  <c:v>73.156862745098053</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>67.352941176470608</c:v>
+                  <c:v>74.725490196078439</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>68.764705882352956</c:v>
+                  <c:v>76.294117647058826</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>70.176470588235304</c:v>
+                  <c:v>77.862745098039213</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>71.588235294117652</c:v>
+                  <c:v>79.431372549019599</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -879,160 +880,160 @@
             <c:numRef>
               <c:f>Клапана!$K$23:$K$73</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="51"/>
                 <c:pt idx="0">
-                  <c:v>15132.293218428747</c:v>
+                  <c:v>16813.699004992479</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15132.375521433616</c:v>
+                  <c:v>16813.842258211898</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15132.293723711138</c:v>
+                  <c:v>16813.715075030814</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15132.351640856588</c:v>
+                  <c:v>16813.760604084378</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15132.380465611186</c:v>
+                  <c:v>16813.694229773246</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15132.306703253296</c:v>
+                  <c:v>16813.674309503742</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15132.315932744956</c:v>
+                  <c:v>16813.670850984254</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15132.364500612437</c:v>
+                  <c:v>16813.6805113665</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>15132.328287327928</c:v>
+                  <c:v>16813.725411472817</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>15132.311802105083</c:v>
+                  <c:v>16813.682360464161</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>15132.428086533779</c:v>
+                  <c:v>16813.734874681959</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>15132.347992396371</c:v>
+                  <c:v>16813.738072703811</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>15132.293614319911</c:v>
+                  <c:v>16813.659679700431</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>15132.293208010435</c:v>
+                  <c:v>16813.659622400184</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>15132.293645574842</c:v>
+                  <c:v>16813.694663263974</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15132.293499720039</c:v>
+                  <c:v>16814.147986490712</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>15132.31637660822</c:v>
+                  <c:v>16813.695087841308</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>15132.406299383623</c:v>
+                  <c:v>16813.684108693684</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>15132.293598692959</c:v>
+                  <c:v>16814.104561307904</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>15132.293890402299</c:v>
+                  <c:v>16813.670382615863</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>15132.293775802431</c:v>
+                  <c:v>16813.677560304779</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>15132.330117306123</c:v>
+                  <c:v>16813.675263479268</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>15132.339364156793</c:v>
+                  <c:v>16814.049529865501</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>15132.444305090065</c:v>
+                  <c:v>16813.671399895844</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>15132.593044874915</c:v>
+                  <c:v>16813.659341109062</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>15132.436227065908</c:v>
+                  <c:v>16813.698182482058</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>15132.317098549966</c:v>
+                  <c:v>16813.691592585339</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>15132.421149090058</c:v>
+                  <c:v>16813.721606360021</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>15123.567390728287</c:v>
+                  <c:v>16805.632134068339</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>15087.823257771033</c:v>
+                  <c:v>16768.087066544456</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>15024.088805923846</c:v>
+                  <c:v>16699.455697083318</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>14931.930165945385</c:v>
+                  <c:v>16599.148005000243</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>14810.117273269569</c:v>
+                  <c:v>16466.323186004869</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>14658.285117179616</c:v>
+                  <c:v>16300.05700211554</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>14475.242195036961</c:v>
+                  <c:v>16099.632646542626</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>14259.812715443462</c:v>
+                  <c:v>15862.240195755601</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>14009.855395414645</c:v>
+                  <c:v>15587.431052089407</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>13723.985036855227</c:v>
+                  <c:v>15272.711926882253</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>13399.611072142128</c:v>
+                  <c:v>14915.35905775203</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>13033.611809348726</c:v>
+                  <c:v>14512.11215391919</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>12622.558699543064</c:v>
+                  <c:v>14059.158646153966</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>12161.862989000681</c:v>
+                  <c:v>13551.462435928721</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>11645.470475847967</c:v>
+                  <c:v>12982.21446456806</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>11065.613139281118</c:v>
+                  <c:v>12343.41439978681</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>10411.738924275027</c:v>
+                  <c:v>11623.203203798777</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>9668.8968073502783</c:v>
+                  <c:v>10805.354143714649</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>8814.4424417758291</c:v>
+                  <c:v>9865.8155885100296</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>7811.9570849652991</c:v>
+                  <c:v>8765.606616439487</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>6594.3921634374619</c:v>
+                  <c:v>7433.4435238243213</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>5007.3796364780646</c:v>
+                  <c:v>5709.6802942768172</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>2406.0122810436478</c:v>
+                  <c:v>2978.052165669671</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1201,7 +1202,7 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>72</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1213,7 +1214,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>14326.055531312555</c:v>
+                  <c:v>16570.563391623593</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1252,238 +1253,238 @@
             <c:numRef>
               <c:f>Клапана!$I$23:$I$99</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="77"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.4117647058823533</c:v>
+                  <c:v>2.5686274509803919</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.8235294117647065</c:v>
+                  <c:v>4.1372549019607838</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.2352941176470598</c:v>
+                  <c:v>5.7058823529411757</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.647058823529413</c:v>
+                  <c:v>7.2745098039215677</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.0588235294117663</c:v>
+                  <c:v>8.8431372549019596</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.4705882352941195</c:v>
+                  <c:v>10.411764705882351</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10.882352941176473</c:v>
+                  <c:v>11.980392156862743</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12.294117647058826</c:v>
+                  <c:v>13.549019607843135</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>13.705882352941179</c:v>
+                  <c:v>15.117647058823527</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>15.117647058823533</c:v>
+                  <c:v>16.686274509803919</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>16.529411764705884</c:v>
+                  <c:v>18.254901960784313</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>17.941176470588236</c:v>
+                  <c:v>19.823529411764707</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>19.352941176470587</c:v>
+                  <c:v>21.3921568627451</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>20.764705882352938</c:v>
+                  <c:v>22.960784313725494</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>22.17647058823529</c:v>
+                  <c:v>24.529411764705888</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>23.588235294117641</c:v>
+                  <c:v>26.098039215686281</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>24.999999999999993</c:v>
+                  <c:v>27.666666666666675</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>26.411764705882344</c:v>
+                  <c:v>29.235294117647069</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>27.823529411764696</c:v>
+                  <c:v>30.803921568627462</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>29.235294117647047</c:v>
+                  <c:v>32.372549019607852</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>30.647058823529399</c:v>
+                  <c:v>33.941176470588246</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>32.058823529411754</c:v>
+                  <c:v>35.50980392156864</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>33.470588235294109</c:v>
+                  <c:v>37.078431372549034</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>34.882352941176464</c:v>
+                  <c:v>38.647058823529427</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>36.294117647058819</c:v>
+                  <c:v>40.215686274509821</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>37.705882352941174</c:v>
+                  <c:v>41.784313725490215</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>39.117647058823529</c:v>
+                  <c:v>43.352941176470608</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>40.529411764705884</c:v>
+                  <c:v>44.921568627451002</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>41.941176470588239</c:v>
+                  <c:v>46.490196078431396</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>43.352941176470594</c:v>
+                  <c:v>48.058823529411789</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>44.764705882352949</c:v>
+                  <c:v>49.627450980392183</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>46.176470588235304</c:v>
+                  <c:v>51.196078431372577</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>47.588235294117659</c:v>
+                  <c:v>52.76470588235297</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>49.000000000000014</c:v>
+                  <c:v>54.333333333333364</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>50.411764705882369</c:v>
+                  <c:v>55.901960784313758</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>51.823529411764724</c:v>
+                  <c:v>57.470588235294152</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>53.235294117647079</c:v>
+                  <c:v>59.039215686274545</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>54.647058823529434</c:v>
+                  <c:v>60.607843137254939</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>56.058823529411789</c:v>
+                  <c:v>62.176470588235333</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>57.470588235294144</c:v>
+                  <c:v>63.745098039215726</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>58.882352941176499</c:v>
+                  <c:v>65.31372549019612</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>60.294117647058854</c:v>
+                  <c:v>66.882352941176507</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>61.705882352941209</c:v>
+                  <c:v>68.450980392156893</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>63.117647058823565</c:v>
+                  <c:v>70.01960784313728</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>64.529411764705912</c:v>
+                  <c:v>71.588235294117666</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>65.94117647058826</c:v>
+                  <c:v>73.156862745098053</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>67.352941176470608</c:v>
+                  <c:v>74.725490196078439</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>68.764705882352956</c:v>
+                  <c:v>76.294117647058826</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>70.176470588235304</c:v>
+                  <c:v>77.862745098039213</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>71.588235294117652</c:v>
+                  <c:v>79.431372549019599</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>73</c:v>
+                  <c:v>80.999999999999986</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>74.411764705882348</c:v>
+                  <c:v>82.568627450980372</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>75.823529411764696</c:v>
+                  <c:v>84.137254901960759</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>77.235294117647044</c:v>
+                  <c:v>85.705882352941146</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>78.647058823529392</c:v>
+                  <c:v>87.274509803921532</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>80.05882352941174</c:v>
+                  <c:v>88.843137254901919</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>81.470588235294088</c:v>
+                  <c:v>90.411764705882305</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>82.882352941176435</c:v>
+                  <c:v>91.980392156862692</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>84.294117647058783</c:v>
+                  <c:v>93.549019607843078</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>85.705882352941131</c:v>
+                  <c:v>95.117647058823465</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>87.117647058823479</c:v>
+                  <c:v>96.686274509803852</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>88.529411764705827</c:v>
+                  <c:v>98.254901960784238</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>89.941176470588175</c:v>
+                  <c:v>99.823529411764625</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>91.352941176470523</c:v>
+                  <c:v>101.39215686274501</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>92.764705882352871</c:v>
+                  <c:v>102.9607843137254</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>94.176470588235219</c:v>
+                  <c:v>104.52941176470578</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>95.588235294117567</c:v>
+                  <c:v>106.09803921568617</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>96.999999999999915</c:v>
+                  <c:v>107.66666666666656</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>98.411764705882263</c:v>
+                  <c:v>109.23529411764694</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>99.823529411764611</c:v>
+                  <c:v>110.80392156862733</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>101.23529411764696</c:v>
+                  <c:v>112.37254901960772</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>102.64705882352931</c:v>
+                  <c:v>113.9411764705881</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>104.05882352941165</c:v>
+                  <c:v>115.50980392156849</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>105.470588235294</c:v>
+                  <c:v>117.07843137254888</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>106.88235294117635</c:v>
+                  <c:v>118.64705882352926</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>108.2941176470587</c:v>
+                  <c:v>120.21568627450965</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1624,106 +1625,106 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0</c:v>
+                  <c:v>13175.682690426402</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0</c:v>
+                  <c:v>13698.503574014099</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0</c:v>
+                  <c:v>14198.306787295387</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0</c:v>
+                  <c:v>14677.541928183915</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>12794.551782045031</c:v>
+                  <c:v>15138.926148343849</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>13282.335488606182</c:v>
+                  <c:v>15581.742943754491</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>13749.522711983491</c:v>
+                  <c:v>16009.926189937602</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>14198.306787296195</c:v>
+                  <c:v>16423.808393728279</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>14630.446737999669</c:v>
+                  <c:v>16824.620411243901</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>15047.369694955658</c:v>
+                  <c:v>17213.340334131321</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>15450.274923663128</c:v>
+                  <c:v>17590.657238765605</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>15844.147396689053</c:v>
+                  <c:v>17957.346134894691</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>16218.518742724234</c:v>
+                  <c:v>18314.234500782801</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>16585.680858167587</c:v>
+                  <c:v>18661.785310102307</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>16942.411442652083</c:v>
+                  <c:v>19000.5934720269</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>17289.614197050938</c:v>
+                  <c:v>19331.587642070772</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>17627.680677787979</c:v>
+                  <c:v>19661.297400586489</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>17957.346134896223</c:v>
+                  <c:v>19990.962848889663</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>18278.854772828065</c:v>
+                  <c:v>20320.6968194492</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>18593.504749915024</c:v>
+                  <c:v>20650.374634433319</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>18899.6877139922</c:v>
+                  <c:v>20980.03300848497</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>19199.901980928051</c:v>
+                  <c:v>21309.880987762608</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>19496.48142348669</c:v>
+                  <c:v>21639.369247559269</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>19793.154075247352</c:v>
+                  <c:v>21969.064307696721</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>20089.929004556132</c:v>
+                  <c:v>22298.704013237257</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>20386.596363812845</c:v>
+                  <c:v>22628.438630814489</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>20683.372066720633</c:v>
+                  <c:v>22958.078409093803</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>20980.03300848461</c:v>
+                  <c:v>23287.754627111255</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>21276.766733582681</c:v>
+                  <c:v>23617.698911038358</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>21573.469266751661</c:v>
+                  <c:v>23947.226282077449</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>21870.245663779282</c:v>
+                  <c:v>24276.781302305331</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>22166.875820776397</c:v>
+                  <c:v>24606.48127580763</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>22463.773442080615</c:v>
+                  <c:v>24936.192523818027</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>22760.290125397136</c:v>
+                  <c:v>25265.959124733825</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1748,238 +1749,238 @@
             <c:numRef>
               <c:f>Клапана!$I$23:$I$99</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="77"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.4117647058823533</c:v>
+                  <c:v>2.5686274509803919</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.8235294117647065</c:v>
+                  <c:v>4.1372549019607838</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.2352941176470598</c:v>
+                  <c:v>5.7058823529411757</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.647058823529413</c:v>
+                  <c:v>7.2745098039215677</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.0588235294117663</c:v>
+                  <c:v>8.8431372549019596</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.4705882352941195</c:v>
+                  <c:v>10.411764705882351</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10.882352941176473</c:v>
+                  <c:v>11.980392156862743</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12.294117647058826</c:v>
+                  <c:v>13.549019607843135</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>13.705882352941179</c:v>
+                  <c:v>15.117647058823527</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>15.117647058823533</c:v>
+                  <c:v>16.686274509803919</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>16.529411764705884</c:v>
+                  <c:v>18.254901960784313</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>17.941176470588236</c:v>
+                  <c:v>19.823529411764707</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>19.352941176470587</c:v>
+                  <c:v>21.3921568627451</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>20.764705882352938</c:v>
+                  <c:v>22.960784313725494</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>22.17647058823529</c:v>
+                  <c:v>24.529411764705888</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>23.588235294117641</c:v>
+                  <c:v>26.098039215686281</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>24.999999999999993</c:v>
+                  <c:v>27.666666666666675</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>26.411764705882344</c:v>
+                  <c:v>29.235294117647069</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>27.823529411764696</c:v>
+                  <c:v>30.803921568627462</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>29.235294117647047</c:v>
+                  <c:v>32.372549019607852</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>30.647058823529399</c:v>
+                  <c:v>33.941176470588246</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>32.058823529411754</c:v>
+                  <c:v>35.50980392156864</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>33.470588235294109</c:v>
+                  <c:v>37.078431372549034</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>34.882352941176464</c:v>
+                  <c:v>38.647058823529427</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>36.294117647058819</c:v>
+                  <c:v>40.215686274509821</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>37.705882352941174</c:v>
+                  <c:v>41.784313725490215</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>39.117647058823529</c:v>
+                  <c:v>43.352941176470608</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>40.529411764705884</c:v>
+                  <c:v>44.921568627451002</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>41.941176470588239</c:v>
+                  <c:v>46.490196078431396</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>43.352941176470594</c:v>
+                  <c:v>48.058823529411789</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>44.764705882352949</c:v>
+                  <c:v>49.627450980392183</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>46.176470588235304</c:v>
+                  <c:v>51.196078431372577</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>47.588235294117659</c:v>
+                  <c:v>52.76470588235297</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>49.000000000000014</c:v>
+                  <c:v>54.333333333333364</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>50.411764705882369</c:v>
+                  <c:v>55.901960784313758</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>51.823529411764724</c:v>
+                  <c:v>57.470588235294152</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>53.235294117647079</c:v>
+                  <c:v>59.039215686274545</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>54.647058823529434</c:v>
+                  <c:v>60.607843137254939</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>56.058823529411789</c:v>
+                  <c:v>62.176470588235333</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>57.470588235294144</c:v>
+                  <c:v>63.745098039215726</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>58.882352941176499</c:v>
+                  <c:v>65.31372549019612</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>60.294117647058854</c:v>
+                  <c:v>66.882352941176507</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>61.705882352941209</c:v>
+                  <c:v>68.450980392156893</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>63.117647058823565</c:v>
+                  <c:v>70.01960784313728</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>64.529411764705912</c:v>
+                  <c:v>71.588235294117666</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>65.94117647058826</c:v>
+                  <c:v>73.156862745098053</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>67.352941176470608</c:v>
+                  <c:v>74.725490196078439</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>68.764705882352956</c:v>
+                  <c:v>76.294117647058826</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>70.176470588235304</c:v>
+                  <c:v>77.862745098039213</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>71.588235294117652</c:v>
+                  <c:v>79.431372549019599</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>73</c:v>
+                  <c:v>80.999999999999986</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>74.411764705882348</c:v>
+                  <c:v>82.568627450980372</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>75.823529411764696</c:v>
+                  <c:v>84.137254901960759</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>77.235294117647044</c:v>
+                  <c:v>85.705882352941146</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>78.647058823529392</c:v>
+                  <c:v>87.274509803921532</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>80.05882352941174</c:v>
+                  <c:v>88.843137254901919</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>81.470588235294088</c:v>
+                  <c:v>90.411764705882305</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>82.882352941176435</c:v>
+                  <c:v>91.980392156862692</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>84.294117647058783</c:v>
+                  <c:v>93.549019607843078</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>85.705882352941131</c:v>
+                  <c:v>95.117647058823465</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>87.117647058823479</c:v>
+                  <c:v>96.686274509803852</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>88.529411764705827</c:v>
+                  <c:v>98.254901960784238</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>89.941176470588175</c:v>
+                  <c:v>99.823529411764625</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>91.352941176470523</c:v>
+                  <c:v>101.39215686274501</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>92.764705882352871</c:v>
+                  <c:v>102.9607843137254</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>94.176470588235219</c:v>
+                  <c:v>104.52941176470578</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>95.588235294117567</c:v>
+                  <c:v>106.09803921568617</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>96.999999999999915</c:v>
+                  <c:v>107.66666666666656</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>98.411764705882263</c:v>
+                  <c:v>109.23529411764694</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>99.823529411764611</c:v>
+                  <c:v>110.80392156862733</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>101.23529411764696</c:v>
+                  <c:v>112.37254901960772</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>102.64705882352931</c:v>
+                  <c:v>113.9411764705881</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>104.05882352941165</c:v>
+                  <c:v>115.50980392156849</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>105.470588235294</c:v>
+                  <c:v>117.07843137254888</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>106.88235294117635</c:v>
+                  <c:v>118.64705882352926</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>108.2941176470587</c:v>
+                  <c:v>120.21568627450965</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2129,97 +2130,97 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0</c:v>
+                  <c:v>14677.541928183915</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0</c:v>
+                  <c:v>15138.926148343849</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0</c:v>
+                  <c:v>15581.742943754491</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0</c:v>
+                  <c:v>16009.926189937602</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0</c:v>
+                  <c:v>16423.808393728279</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>14630.446737999669</c:v>
+                  <c:v>16824.620411243901</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>15047.369694955658</c:v>
+                  <c:v>17213.340334131321</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>15450.274923663128</c:v>
+                  <c:v>17590.657238765605</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>15844.147396689053</c:v>
+                  <c:v>17957.346134894691</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>16218.518742724234</c:v>
+                  <c:v>18314.234500782801</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>16585.680858167587</c:v>
+                  <c:v>18661.785310102307</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>16942.411442652083</c:v>
+                  <c:v>19000.5934720269</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>17289.614197050938</c:v>
+                  <c:v>19331.587642070772</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>17627.680677787979</c:v>
+                  <c:v>19661.297400586489</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>17957.346134896223</c:v>
+                  <c:v>19990.962848889663</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>18278.854772828065</c:v>
+                  <c:v>20320.6968194492</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>18593.504749915024</c:v>
+                  <c:v>20650.374634433319</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>18899.6877139922</c:v>
+                  <c:v>20980.03300848497</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>19199.901980928051</c:v>
+                  <c:v>21309.880987762608</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>19496.48142348669</c:v>
+                  <c:v>21639.369247559269</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>19793.154075247352</c:v>
+                  <c:v>21969.064307696721</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>20089.929004556132</c:v>
+                  <c:v>22298.704013237257</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>20386.596363812845</c:v>
+                  <c:v>22628.438630814489</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>20683.372066720633</c:v>
+                  <c:v>22958.078409093803</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>20980.03300848461</c:v>
+                  <c:v>23287.754627111255</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>21276.766733582681</c:v>
+                  <c:v>23617.698911038358</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>21573.469266751661</c:v>
+                  <c:v>23947.226282077449</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>21870.245663779282</c:v>
+                  <c:v>24276.781302305331</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>22166.875820776397</c:v>
+                  <c:v>24606.48127580763</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>22463.773442080615</c:v>
+                  <c:v>24936.192523818027</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>22760.290125397136</c:v>
+                  <c:v>25265.959124733825</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2444,9 +2445,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office 2013–2022">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2484,7 +2485,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2590,7 +2591,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2732,7 +2733,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2743,8 +2744,8 @@
   <sheetPr codeName="Worksheet____5"/>
   <dimension ref="A1:AD99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
@@ -2768,7 +2769,7 @@
     <col min="31" max="16384" width="9.15234375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="37.299999999999997" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:30" ht="38.15" x14ac:dyDescent="0.4">
       <c r="A1" s="22" t="s">
         <v>41</v>
       </c>
@@ -2781,7 +2782,7 @@
       </c>
       <c r="G1" t="str" cm="1">
         <f t="array" ref="G1">[1]!unf_version()</f>
-        <v>7.49</v>
+        <v>7.50</v>
       </c>
       <c r="H1"/>
       <c r="U1" s="1" t="s">
@@ -2876,12 +2877,12 @@
       </c>
     </row>
     <row r="4" spans="1:30" ht="12.9" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="31"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="25"/>
       <c r="V4" s="1" t="s">
         <v>13</v>
       </c>
@@ -2918,10 +2919,10 @@
       <c r="B5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="33"/>
+      <c r="D5" s="27"/>
       <c r="E5" s="7"/>
       <c r="G5" s="8" t="s">
         <v>32</v>
@@ -2967,10 +2968,10 @@
       <c r="B6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="34"/>
+      <c r="D6" s="28"/>
       <c r="E6" s="9"/>
       <c r="G6" s="8" t="s">
         <v>33</v>
@@ -3018,10 +3019,10 @@
       <c r="B7" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="34"/>
+      <c r="D7" s="28"/>
       <c r="E7" s="9"/>
       <c r="V7" s="1" t="s">
         <v>13</v>
@@ -3059,11 +3060,11 @@
       <c r="B8" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="35">
+      <c r="C8" s="29">
         <f>VLOOKUP(C11,W3:AD7,2,0)</f>
         <v>25.4</v>
       </c>
-      <c r="D8" s="35"/>
+      <c r="D8" s="29"/>
       <c r="E8" s="9" t="s">
         <v>10</v>
       </c>
@@ -3083,10 +3084,10 @@
       <c r="B11" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="25"/>
+      <c r="D11" s="32"/>
       <c r="E11" s="9"/>
       <c r="X11" s="2"/>
       <c r="Y11" s="2"/>
@@ -3095,11 +3096,11 @@
       <c r="B12" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="26">
+      <c r="C12" s="33">
         <f>VLOOKUP(C11,W3:AD7,4,0)</f>
         <v>7.94</v>
       </c>
-      <c r="D12" s="26"/>
+      <c r="D12" s="33"/>
       <c r="E12" s="9" t="s">
         <v>10</v>
       </c>
@@ -3110,11 +3111,11 @@
       <c r="B13" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="26">
+      <c r="C13" s="33">
         <f>VLOOKUP(C11,W3:AD7,6,0)</f>
         <v>0.25805</v>
       </c>
-      <c r="D13" s="26"/>
+      <c r="D13" s="33"/>
       <c r="E13" s="9"/>
       <c r="X13" s="2"/>
       <c r="Y13" s="2"/>
@@ -3153,11 +3154,11 @@
       <c r="B16" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="27">
+      <c r="C16" s="34">
         <f>((C14^2+D14^2+C15^2+D15^2))^(0.5)</f>
         <v>4.2426406871192848</v>
       </c>
-      <c r="D16" s="27"/>
+      <c r="D16" s="34"/>
       <c r="E16" s="9"/>
       <c r="X16" s="2"/>
       <c r="Y16" s="2"/>
@@ -3166,20 +3167,16 @@
       <c r="B17" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="28">
+      <c r="C17" s="35">
         <f>C16</f>
         <v>4.2426406871192848</v>
       </c>
-      <c r="D17" s="28"/>
+      <c r="D17" s="35"/>
       <c r="E17" s="9"/>
       <c r="X17" s="2"/>
       <c r="Y17" s="2"/>
     </row>
     <row r="18" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="G18" s="1" t="e" cm="1">
-        <f t="array" ref="G18">GLV_p</f>
-        <v>#NAME?</v>
-      </c>
       <c r="X18" s="2"/>
       <c r="Y18" s="2"/>
     </row>
@@ -3187,10 +3184,10 @@
       <c r="B19" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="23">
-        <v>72</v>
-      </c>
-      <c r="D19" s="23"/>
+      <c r="C19" s="30">
+        <v>80</v>
+      </c>
+      <c r="D19" s="30"/>
       <c r="E19" s="9" t="s">
         <v>28</v>
       </c>
@@ -3199,10 +3196,10 @@
       <c r="B20" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="24">
+      <c r="C20" s="31">
         <v>50</v>
       </c>
-      <c r="D20" s="24"/>
+      <c r="D20" s="31"/>
       <c r="E20" s="9" t="s">
         <v>28</v>
       </c>
@@ -3213,7 +3210,7 @@
       </c>
       <c r="C21" s="19">
         <f t="array" ref="C21:D27">TRANSPOSE([1]!GLV_p_vkr_atma(C12,C17,C19,C29,H5,H6,1))</f>
-        <v>49.952452966948883</v>
+        <v>49.873546067686959</v>
       </c>
       <c r="D21" s="1" t="str">
         <v>p_atma</v>
@@ -3221,12 +3218,12 @@
       <c r="E21" s="9"/>
       <c r="I21" s="1">
         <f>C19*1</f>
-        <v>72</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="2:25" x14ac:dyDescent="0.3">
       <c r="C22" s="19">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="D22" s="1" t="str">
         <v>p_in_atma</v>
@@ -3234,21 +3231,21 @@
     </row>
     <row r="23" spans="2:25" x14ac:dyDescent="0.3">
       <c r="C23" s="19">
-        <v>70.861251006900801</v>
+        <v>78.652332986652439</v>
       </c>
       <c r="D23" s="1" t="str">
         <v>p_v_atma</v>
       </c>
-      <c r="I23" s="1">
+      <c r="I23" s="36">
         <v>1</v>
       </c>
-      <c r="J23" s="1">
+      <c r="J23" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I23,$H$5,$H$6)/1000</f>
-        <v>15.132293218428748</v>
-      </c>
-      <c r="K23" s="1">
+        <v>16.813699004992479</v>
+      </c>
+      <c r="K23" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I23,$H$5,$H$6)</f>
-        <v>15132.293218428747</v>
+        <v>16813.699004992479</v>
       </c>
       <c r="L23" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I23,$C$20,$H$5,$H$6)</f>
@@ -3265,22 +3262,22 @@
     </row>
     <row r="24" spans="2:25" x14ac:dyDescent="0.3">
       <c r="C24" s="20">
-        <v>49.952452966948883</v>
+        <v>49.873546067686959</v>
       </c>
       <c r="D24" s="1" t="str">
         <v>p_out_atma</v>
       </c>
-      <c r="I24" s="1">
+      <c r="I24" s="36">
         <f>I23+$I$21/51</f>
-        <v>2.4117647058823533</v>
-      </c>
-      <c r="J24" s="1">
+        <v>2.5686274509803919</v>
+      </c>
+      <c r="J24" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I24,$H$5,$H$6)/1000</f>
-        <v>15.132375521433616</v>
-      </c>
-      <c r="K24" s="1">
+        <v>16.813842258211899</v>
+      </c>
+      <c r="K24" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I24,$H$5,$H$6)</f>
-        <v>15132.375521433616</v>
+        <v>16813.842258211898</v>
       </c>
       <c r="L24" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I24,$C$20,$H$5,$H$6)</f>
@@ -3297,22 +3294,22 @@
     </row>
     <row r="25" spans="2:25" x14ac:dyDescent="0.3">
       <c r="C25" s="18">
-        <v>14326.055531312555</v>
+        <v>16570.563391623593</v>
       </c>
       <c r="D25" s="1" t="str">
         <v>q_gas_sm3day</v>
       </c>
-      <c r="I25" s="1">
+      <c r="I25" s="36">
         <f t="shared" ref="I25:I88" si="2">I24+$I$21/51</f>
-        <v>3.8235294117647065</v>
-      </c>
-      <c r="J25" s="1">
+        <v>4.1372549019607838</v>
+      </c>
+      <c r="J25" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I25,$H$5,$H$6)/1000</f>
-        <v>15.132293723711138</v>
-      </c>
-      <c r="K25" s="1">
+        <v>16.813715075030814</v>
+      </c>
+      <c r="K25" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I25,$H$5,$H$6)</f>
-        <v>15132.293723711138</v>
+        <v>16813.715075030814</v>
       </c>
       <c r="L25" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I25,$C$20,$H$5,$H$6)</f>
@@ -3334,17 +3331,17 @@
       <c r="D26" s="1" t="str">
         <v>port critical flow</v>
       </c>
-      <c r="I26" s="1">
-        <f t="shared" si="2"/>
-        <v>5.2352941176470598</v>
-      </c>
-      <c r="J26" s="1">
+      <c r="I26" s="36">
+        <f t="shared" si="2"/>
+        <v>5.7058823529411757</v>
+      </c>
+      <c r="J26" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I26,$H$5,$H$6)/1000</f>
-        <v>15.132351640856589</v>
-      </c>
-      <c r="K26" s="1">
+        <v>16.813760604084379</v>
+      </c>
+      <c r="K26" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I26,$H$5,$H$6)</f>
-        <v>15132.351640856588</v>
+        <v>16813.760604084378</v>
       </c>
       <c r="L26" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I26,$C$20,$H$5,$H$6)</f>
@@ -3366,17 +3363,17 @@
       <c r="D27" s="1" t="str">
         <v>vkrutka critical flow</v>
       </c>
-      <c r="I27" s="1">
-        <f t="shared" si="2"/>
-        <v>6.647058823529413</v>
-      </c>
-      <c r="J27" s="1">
+      <c r="I27" s="36">
+        <f t="shared" si="2"/>
+        <v>7.2745098039215677</v>
+      </c>
+      <c r="J27" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I27,$H$5,$H$6)/1000</f>
-        <v>15.132380465611186</v>
-      </c>
-      <c r="K27" s="1">
+        <v>16.813694229773247</v>
+      </c>
+      <c r="K27" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I27,$H$5,$H$6)</f>
-        <v>15132.380465611186</v>
+        <v>16813.694229773246</v>
       </c>
       <c r="L27" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I27,$C$20,$H$5,$H$6)</f>
@@ -3392,17 +3389,17 @@
       </c>
     </row>
     <row r="28" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="I28" s="1">
-        <f t="shared" si="2"/>
-        <v>8.0588235294117663</v>
-      </c>
-      <c r="J28" s="1">
+      <c r="I28" s="36">
+        <f t="shared" si="2"/>
+        <v>8.8431372549019596</v>
+      </c>
+      <c r="J28" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I28,$H$5,$H$6)/1000</f>
-        <v>15.132306703253295</v>
-      </c>
-      <c r="K28" s="1">
+        <v>16.813674309503742</v>
+      </c>
+      <c r="K28" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I28,$H$5,$H$6)</f>
-        <v>15132.306703253296</v>
+        <v>16813.674309503742</v>
       </c>
       <c r="L28" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I28,$C$20,$H$5,$H$6)</f>
@@ -3423,22 +3420,22 @@
       </c>
       <c r="C29" s="18">
         <f t="array" ref="C29:D35">TRANSPOSE([1]!GLV_q_gas_vkr_sm3day(C12,C17,C19,C20,H5,H6))</f>
-        <v>14326.055531312555</v>
+        <v>16570.563391623593</v>
       </c>
       <c r="D29" s="1" t="str">
         <v>q_gas_sm3day</v>
       </c>
-      <c r="I29" s="1">
-        <f t="shared" si="2"/>
-        <v>9.4705882352941195</v>
-      </c>
-      <c r="J29" s="1">
+      <c r="I29" s="36">
+        <f t="shared" si="2"/>
+        <v>10.411764705882351</v>
+      </c>
+      <c r="J29" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I29,$H$5,$H$6)/1000</f>
-        <v>15.132315932744955</v>
-      </c>
-      <c r="K29" s="1">
+        <v>16.813670850984252</v>
+      </c>
+      <c r="K29" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I29,$H$5,$H$6)</f>
-        <v>15132.315932744956</v>
+        <v>16813.670850984254</v>
       </c>
       <c r="L29" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I29,$C$20,$H$5,$H$6)</f>
@@ -3455,22 +3452,22 @@
     </row>
     <row r="30" spans="2:25" x14ac:dyDescent="0.3">
       <c r="C30" s="19">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="D30" s="1" t="str">
         <v>p_in_atma</v>
       </c>
-      <c r="I30" s="1">
-        <f t="shared" si="2"/>
-        <v>10.882352941176473</v>
-      </c>
-      <c r="J30" s="1">
+      <c r="I30" s="36">
+        <f t="shared" si="2"/>
+        <v>11.980392156862743</v>
+      </c>
+      <c r="J30" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I30,$H$5,$H$6)/1000</f>
-        <v>15.132364500612438</v>
-      </c>
-      <c r="K30" s="1">
+        <v>16.813680511366499</v>
+      </c>
+      <c r="K30" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I30,$H$5,$H$6)</f>
-        <v>15132.364500612437</v>
+        <v>16813.6805113665</v>
       </c>
       <c r="L30" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I30,$C$20,$H$5,$H$6)</f>
@@ -3487,22 +3484,22 @@
     </row>
     <row r="31" spans="2:25" x14ac:dyDescent="0.3">
       <c r="C31" s="19">
-        <v>70.8857512084967</v>
+        <v>78.656142549463681</v>
       </c>
       <c r="D31" s="1" t="str">
         <v>pv_atma</v>
       </c>
-      <c r="I31" s="1">
-        <f t="shared" si="2"/>
-        <v>12.294117647058826</v>
-      </c>
-      <c r="J31" s="1">
+      <c r="I31" s="36">
+        <f t="shared" si="2"/>
+        <v>13.549019607843135</v>
+      </c>
+      <c r="J31" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I31,$H$5,$H$6)/1000</f>
-        <v>15.132328287327928</v>
-      </c>
-      <c r="K31" s="1">
+        <v>16.813725411472817</v>
+      </c>
+      <c r="K31" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I31,$H$5,$H$6)</f>
-        <v>15132.328287327928</v>
+        <v>16813.725411472817</v>
       </c>
       <c r="L31" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I31,$C$20,$H$5,$H$6)</f>
@@ -3524,17 +3521,17 @@
       <c r="D32" s="1" t="str">
         <v>p_out_atma</v>
       </c>
-      <c r="I32" s="1">
-        <f t="shared" si="2"/>
-        <v>13.705882352941179</v>
-      </c>
-      <c r="J32" s="1">
+      <c r="I32" s="36">
+        <f t="shared" si="2"/>
+        <v>15.117647058823527</v>
+      </c>
+      <c r="J32" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I32,$H$5,$H$6)/1000</f>
-        <v>15.132311802105082</v>
-      </c>
-      <c r="K32" s="1">
+        <v>16.81368236046416</v>
+      </c>
+      <c r="K32" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I32,$H$5,$H$6)</f>
-        <v>15132.311802105083</v>
+        <v>16813.682360464161</v>
       </c>
       <c r="L32" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I32,$C$20,$H$5,$H$6)</f>
@@ -3551,22 +3548,22 @@
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C33" s="18">
-        <v>14326.055531312555</v>
+        <v>16570.563391623593</v>
       </c>
       <c r="D33" s="1" t="str">
         <v>q_gas_sm3day</v>
       </c>
-      <c r="I33" s="1">
-        <f t="shared" si="2"/>
-        <v>15.117647058823533</v>
-      </c>
-      <c r="J33" s="1">
+      <c r="I33" s="36">
+        <f t="shared" si="2"/>
+        <v>16.686274509803919</v>
+      </c>
+      <c r="J33" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I33,$H$5,$H$6)/1000</f>
-        <v>15.132428086533778</v>
-      </c>
-      <c r="K33" s="1">
+        <v>16.813734874681959</v>
+      </c>
+      <c r="K33" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I33,$H$5,$H$6)</f>
-        <v>15132.428086533779</v>
+        <v>16813.734874681959</v>
       </c>
       <c r="L33" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I33,$C$20,$H$5,$H$6)</f>
@@ -3588,17 +3585,17 @@
       <c r="D34" s="1" t="str">
         <v>crit1</v>
       </c>
-      <c r="I34" s="1">
-        <f t="shared" si="2"/>
-        <v>16.529411764705884</v>
-      </c>
-      <c r="J34" s="1">
+      <c r="I34" s="36">
+        <f t="shared" si="2"/>
+        <v>18.254901960784313</v>
+      </c>
+      <c r="J34" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I34,$H$5,$H$6)/1000</f>
-        <v>15.132347992396371</v>
-      </c>
-      <c r="K34" s="1">
+        <v>16.81373807270381</v>
+      </c>
+      <c r="K34" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I34,$H$5,$H$6)</f>
-        <v>15132.347992396371</v>
+        <v>16813.738072703811</v>
       </c>
       <c r="L34" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I34,$C$20,$H$5,$H$6)</f>
@@ -3620,17 +3617,17 @@
       <c r="D35" s="1" t="str">
         <v>crit2</v>
       </c>
-      <c r="I35" s="1">
-        <f t="shared" si="2"/>
-        <v>17.941176470588236</v>
-      </c>
-      <c r="J35" s="1">
+      <c r="I35" s="36">
+        <f t="shared" si="2"/>
+        <v>19.823529411764707</v>
+      </c>
+      <c r="J35" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I35,$H$5,$H$6)/1000</f>
-        <v>15.132293614319911</v>
-      </c>
-      <c r="K35" s="1">
+        <v>16.813659679700432</v>
+      </c>
+      <c r="K35" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I35,$H$5,$H$6)</f>
-        <v>15132.293614319911</v>
+        <v>16813.659679700431</v>
       </c>
       <c r="L35" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I35,$C$20,$H$5,$H$6)</f>
@@ -3646,17 +3643,17 @@
       </c>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="I36" s="1">
-        <f t="shared" si="2"/>
-        <v>19.352941176470587</v>
-      </c>
-      <c r="J36" s="1">
+      <c r="I36" s="36">
+        <f t="shared" si="2"/>
+        <v>21.3921568627451</v>
+      </c>
+      <c r="J36" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I36,$H$5,$H$6)/1000</f>
-        <v>15.132293208010434</v>
-      </c>
-      <c r="K36" s="1">
+        <v>16.813659622400184</v>
+      </c>
+      <c r="K36" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I36,$H$5,$H$6)</f>
-        <v>15132.293208010435</v>
+        <v>16813.659622400184</v>
       </c>
       <c r="L36" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I36,$C$20,$H$5,$H$6)</f>
@@ -3682,17 +3679,17 @@
       <c r="E37" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="I37" s="1">
-        <f t="shared" si="2"/>
-        <v>20.764705882352938</v>
-      </c>
-      <c r="J37" s="1">
+      <c r="I37" s="36">
+        <f t="shared" si="2"/>
+        <v>22.960784313725494</v>
+      </c>
+      <c r="J37" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I37,$H$5,$H$6)/1000</f>
-        <v>15.132293645574842</v>
-      </c>
-      <c r="K37" s="1">
+        <v>16.813694663263973</v>
+      </c>
+      <c r="K37" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I37,$H$5,$H$6)</f>
-        <v>15132.293645574842</v>
+        <v>16813.694663263974</v>
       </c>
       <c r="L37" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I37,$C$20,$H$5,$H$6)</f>
@@ -3719,17 +3716,17 @@
       <c r="E38" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="I38" s="1">
-        <f t="shared" si="2"/>
-        <v>22.17647058823529</v>
-      </c>
-      <c r="J38" s="1">
+      <c r="I38" s="36">
+        <f t="shared" si="2"/>
+        <v>24.529411764705888</v>
+      </c>
+      <c r="J38" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I38,$H$5,$H$6)/1000</f>
-        <v>15.132293499720038</v>
-      </c>
-      <c r="K38" s="1">
+        <v>16.814147986490713</v>
+      </c>
+      <c r="K38" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I38,$H$5,$H$6)</f>
-        <v>15132.293499720039</v>
+        <v>16814.147986490712</v>
       </c>
       <c r="L38" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I38,$C$20,$H$5,$H$6)</f>
@@ -3759,17 +3756,17 @@
       <c r="E39" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="I39" s="1">
-        <f t="shared" si="2"/>
-        <v>23.588235294117641</v>
-      </c>
-      <c r="J39" s="1">
+      <c r="I39" s="36">
+        <f t="shared" si="2"/>
+        <v>26.098039215686281</v>
+      </c>
+      <c r="J39" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I39,$H$5,$H$6)/1000</f>
-        <v>15.13231637660822</v>
-      </c>
-      <c r="K39" s="1">
+        <v>16.813695087841307</v>
+      </c>
+      <c r="K39" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I39,$H$5,$H$6)</f>
-        <v>15132.31637660822</v>
+        <v>16813.695087841308</v>
       </c>
       <c r="L39" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I39,$C$20,$H$5,$H$6)</f>
@@ -3799,17 +3796,17 @@
       <c r="E40" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="I40" s="1">
-        <f t="shared" si="2"/>
-        <v>24.999999999999993</v>
-      </c>
-      <c r="J40" s="1">
+      <c r="I40" s="36">
+        <f t="shared" si="2"/>
+        <v>27.666666666666675</v>
+      </c>
+      <c r="J40" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I40,$H$5,$H$6)/1000</f>
-        <v>15.132406299383623</v>
-      </c>
-      <c r="K40" s="1">
+        <v>16.813684108693685</v>
+      </c>
+      <c r="K40" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I40,$H$5,$H$6)</f>
-        <v>15132.406299383623</v>
+        <v>16813.684108693684</v>
       </c>
       <c r="L40" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I40,$C$20,$H$5,$H$6)</f>
@@ -3830,21 +3827,21 @@
       </c>
       <c r="C41" s="21" t="str">
         <f>IF(C19&gt;C40,"открыт",IF(C19&gt;C39,"открыт условно","закрыт"))</f>
-        <v>открыт условно</v>
+        <v>открыт</v>
       </c>
       <c r="D41" s="16"/>
       <c r="E41" s="9"/>
-      <c r="I41" s="1">
-        <f t="shared" si="2"/>
-        <v>26.411764705882344</v>
-      </c>
-      <c r="J41" s="1">
+      <c r="I41" s="36">
+        <f t="shared" si="2"/>
+        <v>29.235294117647069</v>
+      </c>
+      <c r="J41" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I41,$H$5,$H$6)/1000</f>
-        <v>15.132293598692959</v>
-      </c>
-      <c r="K41" s="1">
+        <v>16.814104561307904</v>
+      </c>
+      <c r="K41" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I41,$H$5,$H$6)</f>
-        <v>15132.293598692959</v>
+        <v>16814.104561307904</v>
       </c>
       <c r="L41" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I41,$C$20,$H$5,$H$6)</f>
@@ -3871,17 +3868,17 @@
       <c r="E42" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="I42" s="1">
-        <f t="shared" si="2"/>
-        <v>27.823529411764696</v>
-      </c>
-      <c r="J42" s="1">
+      <c r="I42" s="36">
+        <f t="shared" si="2"/>
+        <v>30.803921568627462</v>
+      </c>
+      <c r="J42" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I42,$H$5,$H$6)/1000</f>
-        <v>15.1322938904023</v>
-      </c>
-      <c r="K42" s="1">
+        <v>16.813670382615864</v>
+      </c>
+      <c r="K42" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I42,$H$5,$H$6)</f>
-        <v>15132.293890402299</v>
+        <v>16813.670382615863</v>
       </c>
       <c r="L42" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I42,$C$20,$H$5,$H$6)</f>
@@ -3901,17 +3898,17 @@
       <c r="C43" s="13"/>
       <c r="D43" s="13"/>
       <c r="E43" s="9"/>
-      <c r="I43" s="1">
-        <f t="shared" si="2"/>
-        <v>29.235294117647047</v>
-      </c>
-      <c r="J43" s="1">
+      <c r="I43" s="36">
+        <f t="shared" si="2"/>
+        <v>32.372549019607852</v>
+      </c>
+      <c r="J43" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I43,$H$5,$H$6)/1000</f>
-        <v>15.132293775802431</v>
-      </c>
-      <c r="K43" s="1">
+        <v>16.813677560304779</v>
+      </c>
+      <c r="K43" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I43,$H$5,$H$6)</f>
-        <v>15132.293775802431</v>
+        <v>16813.677560304779</v>
       </c>
       <c r="L43" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I43,$C$20,$H$5,$H$6)</f>
@@ -3931,17 +3928,17 @@
       <c r="C44" s="13"/>
       <c r="D44" s="13"/>
       <c r="E44" s="9"/>
-      <c r="I44" s="1">
-        <f t="shared" si="2"/>
-        <v>30.647058823529399</v>
-      </c>
-      <c r="J44" s="1">
+      <c r="I44" s="36">
+        <f t="shared" si="2"/>
+        <v>33.941176470588246</v>
+      </c>
+      <c r="J44" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I44,$H$5,$H$6)/1000</f>
-        <v>15.132330117306124</v>
-      </c>
-      <c r="K44" s="1">
+        <v>16.813675263479269</v>
+      </c>
+      <c r="K44" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I44,$H$5,$H$6)</f>
-        <v>15132.330117306123</v>
+        <v>16813.675263479268</v>
       </c>
       <c r="L44" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I44,$C$20,$H$5,$H$6)</f>
@@ -3957,17 +3954,17 @@
       </c>
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="I45" s="1">
-        <f t="shared" si="2"/>
-        <v>32.058823529411754</v>
-      </c>
-      <c r="J45" s="1">
+      <c r="I45" s="36">
+        <f t="shared" si="2"/>
+        <v>35.50980392156864</v>
+      </c>
+      <c r="J45" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I45,$H$5,$H$6)/1000</f>
-        <v>15.132339364156794</v>
-      </c>
-      <c r="K45" s="1">
+        <v>16.8140495298655</v>
+      </c>
+      <c r="K45" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I45,$H$5,$H$6)</f>
-        <v>15132.339364156793</v>
+        <v>16814.049529865501</v>
       </c>
       <c r="L45" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I45,$C$20,$H$5,$H$6)</f>
@@ -3983,17 +3980,17 @@
       </c>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="I46" s="1">
-        <f t="shared" si="2"/>
-        <v>33.470588235294109</v>
-      </c>
-      <c r="J46" s="1">
+      <c r="I46" s="36">
+        <f t="shared" si="2"/>
+        <v>37.078431372549034</v>
+      </c>
+      <c r="J46" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I46,$H$5,$H$6)/1000</f>
-        <v>15.132444305090065</v>
-      </c>
-      <c r="K46" s="1">
+        <v>16.813671399895846</v>
+      </c>
+      <c r="K46" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I46,$H$5,$H$6)</f>
-        <v>15132.444305090065</v>
+        <v>16813.671399895844</v>
       </c>
       <c r="L46" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I46,$C$20,$H$5,$H$6)</f>
@@ -4009,17 +4006,17 @@
       </c>
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="I47" s="1">
-        <f t="shared" si="2"/>
-        <v>34.882352941176464</v>
-      </c>
-      <c r="J47" s="1">
+      <c r="I47" s="36">
+        <f t="shared" si="2"/>
+        <v>38.647058823529427</v>
+      </c>
+      <c r="J47" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I47,$H$5,$H$6)/1000</f>
-        <v>15.132593044874914</v>
-      </c>
-      <c r="K47" s="1">
+        <v>16.813659341109062</v>
+      </c>
+      <c r="K47" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I47,$H$5,$H$6)</f>
-        <v>15132.593044874915</v>
+        <v>16813.659341109062</v>
       </c>
       <c r="L47" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I47,$C$20,$H$5,$H$6)</f>
@@ -4035,17 +4032,17 @@
       </c>
     </row>
     <row r="48" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="I48" s="1">
-        <f t="shared" si="2"/>
-        <v>36.294117647058819</v>
-      </c>
-      <c r="J48" s="1">
+      <c r="I48" s="36">
+        <f t="shared" si="2"/>
+        <v>40.215686274509821</v>
+      </c>
+      <c r="J48" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I48,$H$5,$H$6)/1000</f>
-        <v>15.132436227065908</v>
-      </c>
-      <c r="K48" s="1">
+        <v>16.813698182482057</v>
+      </c>
+      <c r="K48" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I48,$H$5,$H$6)</f>
-        <v>15132.436227065908</v>
+        <v>16813.698182482058</v>
       </c>
       <c r="L48" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I48,$C$20,$H$5,$H$6)</f>
@@ -4061,17 +4058,17 @@
       </c>
     </row>
     <row r="49" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I49" s="1">
-        <f t="shared" si="2"/>
-        <v>37.705882352941174</v>
-      </c>
-      <c r="J49" s="1">
+      <c r="I49" s="36">
+        <f t="shared" si="2"/>
+        <v>41.784313725490215</v>
+      </c>
+      <c r="J49" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I49,$H$5,$H$6)/1000</f>
-        <v>15.132317098549965</v>
-      </c>
-      <c r="K49" s="1">
+        <v>16.813691592585339</v>
+      </c>
+      <c r="K49" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I49,$H$5,$H$6)</f>
-        <v>15132.317098549966</v>
+        <v>16813.691592585339</v>
       </c>
       <c r="L49" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I49,$C$20,$H$5,$H$6)</f>
@@ -4087,17 +4084,17 @@
       </c>
     </row>
     <row r="50" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I50" s="1">
-        <f t="shared" si="2"/>
-        <v>39.117647058823529</v>
-      </c>
-      <c r="J50" s="1">
+      <c r="I50" s="36">
+        <f t="shared" si="2"/>
+        <v>43.352941176470608</v>
+      </c>
+      <c r="J50" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I50,$H$5,$H$6)/1000</f>
-        <v>15.132421149090058</v>
-      </c>
-      <c r="K50" s="1">
+        <v>16.813721606360019</v>
+      </c>
+      <c r="K50" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I50,$H$5,$H$6)</f>
-        <v>15132.421149090058</v>
+        <v>16813.721606360021</v>
       </c>
       <c r="L50" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I50,$C$20,$H$5,$H$6)</f>
@@ -4113,17 +4110,17 @@
       </c>
     </row>
     <row r="51" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I51" s="1">
-        <f t="shared" si="2"/>
-        <v>40.529411764705884</v>
-      </c>
-      <c r="J51" s="1">
+      <c r="I51" s="36">
+        <f t="shared" si="2"/>
+        <v>44.921568627451002</v>
+      </c>
+      <c r="J51" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I51,$H$5,$H$6)/1000</f>
-        <v>15.123567390728287</v>
-      </c>
-      <c r="K51" s="1">
+        <v>16.80563213406834</v>
+      </c>
+      <c r="K51" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I51,$H$5,$H$6)</f>
-        <v>15123.567390728287</v>
+        <v>16805.632134068339</v>
       </c>
       <c r="L51" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I51,$C$20,$H$5,$H$6)</f>
@@ -4139,17 +4136,17 @@
       </c>
     </row>
     <row r="52" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I52" s="1">
-        <f t="shared" si="2"/>
-        <v>41.941176470588239</v>
-      </c>
-      <c r="J52" s="1">
+      <c r="I52" s="36">
+        <f t="shared" si="2"/>
+        <v>46.490196078431396</v>
+      </c>
+      <c r="J52" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I52,$H$5,$H$6)/1000</f>
-        <v>15.087823257771033</v>
-      </c>
-      <c r="K52" s="1">
+        <v>16.768087066544457</v>
+      </c>
+      <c r="K52" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I52,$H$5,$H$6)</f>
-        <v>15087.823257771033</v>
+        <v>16768.087066544456</v>
       </c>
       <c r="L52" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I52,$C$20,$H$5,$H$6)</f>
@@ -4165,17 +4162,17 @@
       </c>
     </row>
     <row r="53" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I53" s="1">
-        <f t="shared" si="2"/>
-        <v>43.352941176470594</v>
-      </c>
-      <c r="J53" s="1">
+      <c r="I53" s="36">
+        <f t="shared" si="2"/>
+        <v>48.058823529411789</v>
+      </c>
+      <c r="J53" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I53,$H$5,$H$6)/1000</f>
-        <v>15.024088805923846</v>
-      </c>
-      <c r="K53" s="1">
+        <v>16.699455697083319</v>
+      </c>
+      <c r="K53" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I53,$H$5,$H$6)</f>
-        <v>15024.088805923846</v>
+        <v>16699.455697083318</v>
       </c>
       <c r="L53" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I53,$C$20,$H$5,$H$6)</f>
@@ -4191,17 +4188,17 @@
       </c>
     </row>
     <row r="54" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I54" s="1">
-        <f t="shared" si="2"/>
-        <v>44.764705882352949</v>
-      </c>
-      <c r="J54" s="1">
+      <c r="I54" s="36">
+        <f t="shared" si="2"/>
+        <v>49.627450980392183</v>
+      </c>
+      <c r="J54" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I54,$H$5,$H$6)/1000</f>
-        <v>14.931930165945385</v>
-      </c>
-      <c r="K54" s="1">
+        <v>16.599148005000242</v>
+      </c>
+      <c r="K54" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I54,$H$5,$H$6)</f>
-        <v>14931.930165945385</v>
+        <v>16599.148005000243</v>
       </c>
       <c r="L54" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I54,$C$20,$H$5,$H$6)</f>
@@ -4217,21 +4214,21 @@
       </c>
     </row>
     <row r="55" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I55" s="1">
-        <f t="shared" si="2"/>
-        <v>46.176470588235304</v>
-      </c>
-      <c r="J55" s="1">
+      <c r="I55" s="36">
+        <f t="shared" si="2"/>
+        <v>51.196078431372577</v>
+      </c>
+      <c r="J55" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I55,$H$5,$H$6)/1000</f>
-        <v>14.810117273269569</v>
-      </c>
-      <c r="K55" s="1">
+        <v>16.466323186004868</v>
+      </c>
+      <c r="K55" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I55,$H$5,$H$6)</f>
-        <v>14810.117273269569</v>
+        <v>16466.323186004869</v>
       </c>
       <c r="L55" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I55,$C$20,$H$5,$H$6)</f>
-        <v>0</v>
+        <v>3423.4923929070064</v>
       </c>
       <c r="M55" s="1">
         <f t="shared" ref="M55:M86" si="3">IF(I55&gt;$C$40,L55,0)</f>
@@ -4243,21 +4240,21 @@
       </c>
     </row>
     <row r="56" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I56" s="1">
-        <f t="shared" si="2"/>
-        <v>47.588235294117659</v>
-      </c>
-      <c r="J56" s="1">
+      <c r="I56" s="36">
+        <f t="shared" si="2"/>
+        <v>52.76470588235297</v>
+      </c>
+      <c r="J56" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I56,$H$5,$H$6)/1000</f>
-        <v>14.658285117179615</v>
-      </c>
-      <c r="K56" s="1">
+        <v>16.30005700211554</v>
+      </c>
+      <c r="K56" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I56,$H$5,$H$6)</f>
-        <v>14658.285117179616</v>
+        <v>16300.05700211554</v>
       </c>
       <c r="L56" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I56,$C$20,$H$5,$H$6)</f>
-        <v>0</v>
+        <v>5197.2993001872655</v>
       </c>
       <c r="M56" s="1">
         <f t="shared" si="3"/>
@@ -4269,21 +4266,21 @@
       </c>
     </row>
     <row r="57" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I57" s="1">
-        <f t="shared" si="2"/>
-        <v>49.000000000000014</v>
-      </c>
-      <c r="J57" s="1">
+      <c r="I57" s="36">
+        <f t="shared" si="2"/>
+        <v>54.333333333333364</v>
+      </c>
+      <c r="J57" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I57,$H$5,$H$6)/1000</f>
-        <v>14.475242195036961</v>
-      </c>
-      <c r="K57" s="1">
+        <v>16.099632646542627</v>
+      </c>
+      <c r="K57" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I57,$H$5,$H$6)</f>
-        <v>14475.242195036961</v>
+        <v>16099.632646542626</v>
       </c>
       <c r="L57" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I57,$C$20,$H$5,$H$6)</f>
-        <v>0</v>
+        <v>6493.0383787717783</v>
       </c>
       <c r="M57" s="1">
         <f t="shared" si="3"/>
@@ -4295,21 +4292,21 @@
       </c>
     </row>
     <row r="58" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I58" s="1">
-        <f t="shared" si="2"/>
-        <v>50.411764705882369</v>
-      </c>
-      <c r="J58" s="1">
+      <c r="I58" s="36">
+        <f t="shared" si="2"/>
+        <v>55.901960784313758</v>
+      </c>
+      <c r="J58" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I58,$H$5,$H$6)/1000</f>
-        <v>14.259812715443463</v>
-      </c>
-      <c r="K58" s="1">
+        <v>15.862240195755602</v>
+      </c>
+      <c r="K58" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I58,$H$5,$H$6)</f>
-        <v>14259.812715443462</v>
+        <v>15862.240195755601</v>
       </c>
       <c r="L58" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I58,$C$20,$H$5,$H$6)</f>
-        <v>2010.489179858429</v>
+        <v>7563.9909144229787</v>
       </c>
       <c r="M58" s="1">
         <f t="shared" si="3"/>
@@ -4321,21 +4318,21 @@
       </c>
     </row>
     <row r="59" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I59" s="1">
-        <f t="shared" si="2"/>
-        <v>51.823529411764724</v>
-      </c>
-      <c r="J59" s="1">
+      <c r="I59" s="36">
+        <f t="shared" si="2"/>
+        <v>57.470588235294152</v>
+      </c>
+      <c r="J59" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I59,$H$5,$H$6)/1000</f>
-        <v>14.009855395414645</v>
-      </c>
-      <c r="K59" s="1">
+        <v>15.587431052089407</v>
+      </c>
+      <c r="K59" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I59,$H$5,$H$6)</f>
-        <v>14009.855395414645</v>
+        <v>15587.431052089407</v>
       </c>
       <c r="L59" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I59,$C$20,$H$5,$H$6)</f>
-        <v>4224.1429980100538</v>
+        <v>8494.2695361295919</v>
       </c>
       <c r="M59" s="1">
         <f t="shared" si="3"/>
@@ -4347,21 +4344,21 @@
       </c>
     </row>
     <row r="60" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I60" s="1">
-        <f t="shared" si="2"/>
-        <v>53.235294117647079</v>
-      </c>
-      <c r="J60" s="1">
+      <c r="I60" s="36">
+        <f t="shared" si="2"/>
+        <v>59.039215686274545</v>
+      </c>
+      <c r="J60" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I60,$H$5,$H$6)/1000</f>
-        <v>13.723985036855227</v>
-      </c>
-      <c r="K60" s="1">
+        <v>15.272711926882254</v>
+      </c>
+      <c r="K60" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I60,$H$5,$H$6)</f>
-        <v>13723.985036855227</v>
+        <v>15272.711926882253</v>
       </c>
       <c r="L60" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I60,$C$20,$H$5,$H$6)</f>
-        <v>5617.5065273126429</v>
+        <v>9326.3010104635869</v>
       </c>
       <c r="M60" s="1">
         <f t="shared" si="3"/>
@@ -4373,21 +4370,21 @@
       </c>
     </row>
     <row r="61" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I61" s="1">
-        <f t="shared" si="2"/>
-        <v>54.647058823529434</v>
-      </c>
-      <c r="J61" s="1">
+      <c r="I61" s="36">
+        <f t="shared" si="2"/>
+        <v>60.607843137254939</v>
+      </c>
+      <c r="J61" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I61,$H$5,$H$6)/1000</f>
-        <v>13.399611072142129</v>
-      </c>
-      <c r="K61" s="1">
+        <v>14.915359057752029</v>
+      </c>
+      <c r="K61" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I61,$H$5,$H$6)</f>
-        <v>13399.611072142128</v>
+        <v>14915.35905775203</v>
       </c>
       <c r="L61" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I61,$C$20,$H$5,$H$6)</f>
-        <v>6721.5078792603445</v>
+        <v>10084.481208458328</v>
       </c>
       <c r="M61" s="1">
         <f t="shared" si="3"/>
@@ -4399,21 +4396,21 @@
       </c>
     </row>
     <row r="62" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I62" s="1">
-        <f t="shared" si="2"/>
-        <v>56.058823529411789</v>
-      </c>
-      <c r="J62" s="1">
+      <c r="I62" s="36">
+        <f t="shared" si="2"/>
+        <v>62.176470588235333</v>
+      </c>
+      <c r="J62" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I62,$H$5,$H$6)/1000</f>
-        <v>13.033611809348725</v>
-      </c>
-      <c r="K62" s="1">
+        <v>14.51211215391919</v>
+      </c>
+      <c r="K62" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I62,$H$5,$H$6)</f>
-        <v>13033.611809348726</v>
+        <v>14512.11215391919</v>
       </c>
       <c r="L62" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I62,$C$20,$H$5,$H$6)</f>
-        <v>7662.4475042268123</v>
+        <v>10784.163208623138</v>
       </c>
       <c r="M62" s="1">
         <f t="shared" si="3"/>
@@ -4425,21 +4422,21 @@
       </c>
     </row>
     <row r="63" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I63" s="1">
-        <f t="shared" si="2"/>
-        <v>57.470588235294144</v>
-      </c>
-      <c r="J63" s="1">
+      <c r="I63" s="36">
+        <f t="shared" si="2"/>
+        <v>63.745098039215726</v>
+      </c>
+      <c r="J63" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I63,$H$5,$H$6)/1000</f>
-        <v>12.622558699543063</v>
-      </c>
-      <c r="K63" s="1">
+        <v>14.059158646153966</v>
+      </c>
+      <c r="K63" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I63,$H$5,$H$6)</f>
-        <v>12622.558699543064</v>
+        <v>14059.158646153966</v>
       </c>
       <c r="L63" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I63,$C$20,$H$5,$H$6)</f>
-        <v>8494.2695361293008</v>
+        <v>11436.292746883195</v>
       </c>
       <c r="M63" s="1">
         <f t="shared" si="3"/>
@@ -4451,21 +4448,21 @@
       </c>
     </row>
     <row r="64" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I64" s="1">
-        <f t="shared" si="2"/>
-        <v>58.882352941176499</v>
-      </c>
-      <c r="J64" s="1">
+      <c r="I64" s="36">
+        <f t="shared" si="2"/>
+        <v>65.31372549019612</v>
+      </c>
+      <c r="J64" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I64,$H$5,$H$6)/1000</f>
-        <v>12.161862989000682</v>
-      </c>
-      <c r="K64" s="1">
+        <v>13.551462435928721</v>
+      </c>
+      <c r="K64" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I64,$H$5,$H$6)</f>
-        <v>12161.862989000681</v>
+        <v>13551.462435928721</v>
       </c>
       <c r="L64" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I64,$C$20,$H$5,$H$6)</f>
-        <v>9246.8116227220344</v>
+        <v>12048.680018828061</v>
       </c>
       <c r="M64" s="1">
         <f t="shared" si="3"/>
@@ -4477,21 +4474,21 @@
       </c>
     </row>
     <row r="65" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I65" s="1">
-        <f t="shared" si="2"/>
-        <v>60.294117647058854</v>
-      </c>
-      <c r="J65" s="1">
+      <c r="I65" s="36">
+        <f t="shared" si="2"/>
+        <v>66.882352941176507</v>
+      </c>
+      <c r="J65" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I65,$H$5,$H$6)/1000</f>
-        <v>11.645470475847967</v>
-      </c>
-      <c r="K65" s="1">
+        <v>12.982214464568059</v>
+      </c>
+      <c r="K65" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I65,$H$5,$H$6)</f>
-        <v>11645.470475847967</v>
+        <v>12982.21446456806</v>
       </c>
       <c r="L65" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I65,$C$20,$H$5,$H$6)</f>
-        <v>9937.9309340547898</v>
+        <v>12627.01386360275</v>
       </c>
       <c r="M65" s="1">
         <f t="shared" si="3"/>
@@ -4503,21 +4500,21 @@
       </c>
     </row>
     <row r="66" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I66" s="1">
-        <f t="shared" si="2"/>
-        <v>61.705882352941209</v>
-      </c>
-      <c r="J66" s="1">
+      <c r="I66" s="36">
+        <f t="shared" si="2"/>
+        <v>68.450980392156893</v>
+      </c>
+      <c r="J66" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I66,$H$5,$H$6)/1000</f>
-        <v>11.065613139281119</v>
-      </c>
-      <c r="K66" s="1">
+        <v>12.343414399786811</v>
+      </c>
+      <c r="K66" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I66,$H$5,$H$6)</f>
-        <v>11065.613139281118</v>
+        <v>12343.41439978681</v>
       </c>
       <c r="L66" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I66,$C$20,$H$5,$H$6)</f>
-        <v>10579.655322593395</v>
+        <v>13175.682690426402</v>
       </c>
       <c r="M66" s="1">
         <f t="shared" si="3"/>
@@ -4525,25 +4522,25 @@
       </c>
       <c r="N66" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>13175.682690426402</v>
       </c>
     </row>
     <row r="67" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I67" s="1">
-        <f t="shared" si="2"/>
-        <v>63.117647058823565</v>
-      </c>
-      <c r="J67" s="1">
+      <c r="I67" s="36">
+        <f t="shared" si="2"/>
+        <v>70.01960784313728</v>
+      </c>
+      <c r="J67" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I67,$H$5,$H$6)/1000</f>
-        <v>10.411738924275026</v>
-      </c>
-      <c r="K67" s="1">
+        <v>11.623203203798777</v>
+      </c>
+      <c r="K67" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I67,$H$5,$H$6)</f>
-        <v>10411.738924275027</v>
+        <v>11623.203203798777</v>
       </c>
       <c r="L67" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I67,$C$20,$H$5,$H$6)</f>
-        <v>11180.613996804726</v>
+        <v>13698.503574014099</v>
       </c>
       <c r="M67" s="1">
         <f t="shared" si="3"/>
@@ -4551,25 +4548,25 @@
       </c>
       <c r="N67" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>13698.503574014099</v>
       </c>
     </row>
     <row r="68" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I68" s="1">
-        <f t="shared" si="2"/>
-        <v>64.529411764705912</v>
-      </c>
-      <c r="J68" s="1">
+      <c r="I68" s="36">
+        <f t="shared" si="2"/>
+        <v>71.588235294117666</v>
+      </c>
+      <c r="J68" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I68,$H$5,$H$6)/1000</f>
-        <v>9.6688968073502775</v>
-      </c>
-      <c r="K68" s="1">
+        <v>10.805354143714649</v>
+      </c>
+      <c r="K68" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I68,$H$5,$H$6)</f>
-        <v>9668.8968073502783</v>
+        <v>10805.354143714649</v>
       </c>
       <c r="L68" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I68,$C$20,$H$5,$H$6)</f>
-        <v>11747.101303961043</v>
+        <v>14198.306787295387</v>
       </c>
       <c r="M68" s="1">
         <f t="shared" si="3"/>
@@ -4577,822 +4574,817 @@
       </c>
       <c r="N68" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>14198.306787295387</v>
       </c>
     </row>
     <row r="69" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I69" s="1">
-        <f t="shared" si="2"/>
-        <v>65.94117647058826</v>
-      </c>
-      <c r="J69" s="1">
+      <c r="I69" s="36">
+        <f t="shared" si="2"/>
+        <v>73.156862745098053</v>
+      </c>
+      <c r="J69" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I69,$H$5,$H$6)/1000</f>
-        <v>8.8144424417758298</v>
-      </c>
-      <c r="K69" s="1">
+        <v>9.8658155885100296</v>
+      </c>
+      <c r="K69" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I69,$H$5,$H$6)</f>
-        <v>8814.4424417758291</v>
+        <v>9865.8155885100296</v>
       </c>
       <c r="L69" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I69,$C$20,$H$5,$H$6)</f>
-        <v>12283.694167692433</v>
+        <v>14677.541928183915</v>
       </c>
       <c r="M69" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>14677.541928183915</v>
       </c>
       <c r="N69" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>14677.541928183915</v>
       </c>
     </row>
     <row r="70" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I70" s="1">
-        <f t="shared" si="2"/>
-        <v>67.352941176470608</v>
-      </c>
-      <c r="J70" s="1">
+      <c r="I70" s="36">
+        <f t="shared" si="2"/>
+        <v>74.725490196078439</v>
+      </c>
+      <c r="J70" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I70,$H$5,$H$6)/1000</f>
-        <v>7.8119570849652993</v>
-      </c>
-      <c r="K70" s="1">
+        <v>8.7656066164394861</v>
+      </c>
+      <c r="K70" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I70,$H$5,$H$6)</f>
-        <v>7811.9570849652991</v>
+        <v>8765.606616439487</v>
       </c>
       <c r="L70" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I70,$C$20,$H$5,$H$6)</f>
-        <v>12794.551782045031</v>
+        <v>15138.926148343849</v>
       </c>
       <c r="M70" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>15138.926148343849</v>
       </c>
       <c r="N70" s="1">
         <f t="shared" si="4"/>
-        <v>12794.551782045031</v>
+        <v>15138.926148343849</v>
       </c>
     </row>
     <row r="71" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I71" s="1">
-        <f t="shared" si="2"/>
-        <v>68.764705882352956</v>
-      </c>
-      <c r="J71" s="1">
+      <c r="I71" s="36">
+        <f t="shared" si="2"/>
+        <v>76.294117647058826</v>
+      </c>
+      <c r="J71" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I71,$H$5,$H$6)/1000</f>
-        <v>6.5943921634374618</v>
-      </c>
-      <c r="K71" s="1">
+        <v>7.4334435238243213</v>
+      </c>
+      <c r="K71" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I71,$H$5,$H$6)</f>
-        <v>6594.3921634374619</v>
+        <v>7433.4435238243213</v>
       </c>
       <c r="L71" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I71,$C$20,$H$5,$H$6)</f>
-        <v>13282.335488606182</v>
+        <v>15581.742943754491</v>
       </c>
       <c r="M71" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>15581.742943754491</v>
       </c>
       <c r="N71" s="1">
         <f t="shared" si="4"/>
-        <v>13282.335488606182</v>
+        <v>15581.742943754491</v>
       </c>
     </row>
     <row r="72" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I72" s="1">
-        <f t="shared" si="2"/>
-        <v>70.176470588235304</v>
-      </c>
-      <c r="J72" s="1">
+      <c r="I72" s="36">
+        <f t="shared" si="2"/>
+        <v>77.862745098039213</v>
+      </c>
+      <c r="J72" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I72,$H$5,$H$6)/1000</f>
-        <v>5.0073796364780643</v>
-      </c>
-      <c r="K72" s="1">
+        <v>5.7096802942768168</v>
+      </c>
+      <c r="K72" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I72,$H$5,$H$6)</f>
-        <v>5007.3796364780646</v>
+        <v>5709.6802942768172</v>
       </c>
       <c r="L72" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I72,$C$20,$H$5,$H$6)</f>
-        <v>13749.522711983491</v>
+        <v>16009.926189937602</v>
       </c>
       <c r="M72" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>16009.926189937602</v>
       </c>
       <c r="N72" s="1">
         <f t="shared" si="4"/>
-        <v>13749.522711983491</v>
+        <v>16009.926189937602</v>
       </c>
     </row>
     <row r="73" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I73" s="1">
-        <f t="shared" si="2"/>
-        <v>71.588235294117652</v>
-      </c>
-      <c r="J73" s="1">
+      <c r="I73" s="36">
+        <f t="shared" si="2"/>
+        <v>79.431372549019599</v>
+      </c>
+      <c r="J73" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I73,$H$5,$H$6)/1000</f>
-        <v>2.4060122810436479</v>
-      </c>
-      <c r="K73" s="1">
+        <v>2.9780521656696708</v>
+      </c>
+      <c r="K73" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I73,$H$5,$H$6)</f>
-        <v>2406.0122810436478</v>
+        <v>2978.052165669671</v>
       </c>
       <c r="L73" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I73,$C$20,$H$5,$H$6)</f>
-        <v>14198.306787296195</v>
+        <v>16423.808393728279</v>
       </c>
       <c r="M73" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>16423.808393728279</v>
       </c>
       <c r="N73" s="1">
         <f t="shared" si="4"/>
-        <v>14198.306787296195</v>
+        <v>16423.808393728279</v>
       </c>
     </row>
     <row r="74" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I74" s="1">
-        <f t="shared" si="2"/>
-        <v>73</v>
-      </c>
-      <c r="J74" s="1">
+      <c r="I74" s="36">
+        <f t="shared" si="2"/>
+        <v>80.999999999999986</v>
+      </c>
+      <c r="J74" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I74,$H$5,$H$6)/1000</f>
         <v>0</v>
       </c>
-      <c r="K74" s="1">
+      <c r="K74" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I74,$H$5,$H$6)</f>
         <v>0</v>
       </c>
       <c r="L74" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I74,$C$20,$H$5,$H$6)</f>
-        <v>14630.446737999669</v>
+        <v>16824.620411243901</v>
       </c>
       <c r="M74" s="1">
         <f t="shared" si="3"/>
-        <v>14630.446737999669</v>
+        <v>16824.620411243901</v>
       </c>
       <c r="N74" s="1">
         <f t="shared" si="4"/>
-        <v>14630.446737999669</v>
+        <v>16824.620411243901</v>
       </c>
     </row>
     <row r="75" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I75" s="1">
-        <f t="shared" si="2"/>
-        <v>74.411764705882348</v>
-      </c>
-      <c r="J75" s="1">
+      <c r="I75" s="36">
+        <f t="shared" si="2"/>
+        <v>82.568627450980372</v>
+      </c>
+      <c r="J75" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I75,$H$5,$H$6)/1000</f>
         <v>0</v>
       </c>
-      <c r="K75" s="1">
+      <c r="K75" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I75,$H$5,$H$6)</f>
         <v>0</v>
       </c>
       <c r="L75" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I75,$C$20,$H$5,$H$6)</f>
-        <v>15047.369694955658</v>
+        <v>17213.340334131321</v>
       </c>
       <c r="M75" s="1">
         <f t="shared" si="3"/>
-        <v>15047.369694955658</v>
+        <v>17213.340334131321</v>
       </c>
       <c r="N75" s="1">
         <f t="shared" si="4"/>
-        <v>15047.369694955658</v>
+        <v>17213.340334131321</v>
       </c>
     </row>
     <row r="76" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I76" s="1">
-        <f t="shared" si="2"/>
-        <v>75.823529411764696</v>
-      </c>
-      <c r="J76" s="1">
+      <c r="I76" s="36">
+        <f t="shared" si="2"/>
+        <v>84.137254901960759</v>
+      </c>
+      <c r="J76" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I76,$H$5,$H$6)/1000</f>
         <v>0</v>
       </c>
-      <c r="K76" s="1">
+      <c r="K76" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I76,$H$5,$H$6)</f>
         <v>0</v>
       </c>
       <c r="L76" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I76,$C$20,$H$5,$H$6)</f>
-        <v>15450.274923663128</v>
+        <v>17590.657238765605</v>
       </c>
       <c r="M76" s="1">
         <f t="shared" si="3"/>
-        <v>15450.274923663128</v>
+        <v>17590.657238765605</v>
       </c>
       <c r="N76" s="1">
         <f t="shared" si="4"/>
-        <v>15450.274923663128</v>
+        <v>17590.657238765605</v>
       </c>
     </row>
     <row r="77" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I77" s="1">
-        <f t="shared" si="2"/>
-        <v>77.235294117647044</v>
-      </c>
-      <c r="J77" s="1">
+      <c r="I77" s="36">
+        <f t="shared" si="2"/>
+        <v>85.705882352941146</v>
+      </c>
+      <c r="J77" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I77,$H$5,$H$6)/1000</f>
         <v>0</v>
       </c>
-      <c r="K77" s="1">
+      <c r="K77" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I77,$H$5,$H$6)</f>
         <v>0</v>
       </c>
       <c r="L77" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I77,$C$20,$H$5,$H$6)</f>
-        <v>15844.147396689053</v>
+        <v>17957.346134894691</v>
       </c>
       <c r="M77" s="1">
         <f t="shared" si="3"/>
-        <v>15844.147396689053</v>
+        <v>17957.346134894691</v>
       </c>
       <c r="N77" s="1">
         <f t="shared" si="4"/>
-        <v>15844.147396689053</v>
+        <v>17957.346134894691</v>
       </c>
     </row>
     <row r="78" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I78" s="1">
-        <f t="shared" si="2"/>
-        <v>78.647058823529392</v>
-      </c>
-      <c r="J78" s="1">
+      <c r="I78" s="36">
+        <f t="shared" si="2"/>
+        <v>87.274509803921532</v>
+      </c>
+      <c r="J78" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I78,$H$5,$H$6)/1000</f>
         <v>0</v>
       </c>
-      <c r="K78" s="1">
+      <c r="K78" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I78,$H$5,$H$6)</f>
         <v>0</v>
       </c>
       <c r="L78" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I78,$C$20,$H$5,$H$6)</f>
-        <v>16218.518742724234</v>
+        <v>18314.234500782801</v>
       </c>
       <c r="M78" s="1">
         <f t="shared" si="3"/>
-        <v>16218.518742724234</v>
+        <v>18314.234500782801</v>
       </c>
       <c r="N78" s="1">
         <f t="shared" si="4"/>
-        <v>16218.518742724234</v>
+        <v>18314.234500782801</v>
       </c>
     </row>
     <row r="79" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I79" s="1">
-        <f t="shared" si="2"/>
-        <v>80.05882352941174</v>
-      </c>
-      <c r="J79" s="1">
+      <c r="I79" s="36">
+        <f t="shared" si="2"/>
+        <v>88.843137254901919</v>
+      </c>
+      <c r="J79" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I79,$H$5,$H$6)/1000</f>
         <v>0</v>
       </c>
-      <c r="K79" s="1">
+      <c r="K79" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I79,$H$5,$H$6)</f>
         <v>0</v>
       </c>
       <c r="L79" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I79,$C$20,$H$5,$H$6)</f>
-        <v>16585.680858167587</v>
+        <v>18661.785310102307</v>
       </c>
       <c r="M79" s="1">
         <f t="shared" si="3"/>
-        <v>16585.680858167587</v>
+        <v>18661.785310102307</v>
       </c>
       <c r="N79" s="1">
         <f t="shared" si="4"/>
-        <v>16585.680858167587</v>
+        <v>18661.785310102307</v>
       </c>
     </row>
     <row r="80" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I80" s="1">
-        <f t="shared" si="2"/>
-        <v>81.470588235294088</v>
-      </c>
-      <c r="J80" s="1">
+      <c r="I80" s="36">
+        <f t="shared" si="2"/>
+        <v>90.411764705882305</v>
+      </c>
+      <c r="J80" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I80,$H$5,$H$6)/1000</f>
         <v>0</v>
       </c>
-      <c r="K80" s="1">
+      <c r="K80" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I80,$H$5,$H$6)</f>
         <v>0</v>
       </c>
       <c r="L80" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I80,$C$20,$H$5,$H$6)</f>
-        <v>16942.411442652083</v>
+        <v>19000.5934720269</v>
       </c>
       <c r="M80" s="1">
         <f t="shared" si="3"/>
-        <v>16942.411442652083</v>
+        <v>19000.5934720269</v>
       </c>
       <c r="N80" s="1">
         <f t="shared" si="4"/>
-        <v>16942.411442652083</v>
+        <v>19000.5934720269</v>
       </c>
     </row>
     <row r="81" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I81" s="1">
-        <f t="shared" si="2"/>
-        <v>82.882352941176435</v>
-      </c>
-      <c r="J81" s="1">
+      <c r="I81" s="36">
+        <f t="shared" si="2"/>
+        <v>91.980392156862692</v>
+      </c>
+      <c r="J81" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I81,$H$5,$H$6)/1000</f>
         <v>0</v>
       </c>
-      <c r="K81" s="1">
+      <c r="K81" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I81,$H$5,$H$6)</f>
         <v>0</v>
       </c>
       <c r="L81" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I81,$C$20,$H$5,$H$6)</f>
-        <v>17289.614197050938</v>
+        <v>19331.587642070772</v>
       </c>
       <c r="M81" s="1">
         <f t="shared" si="3"/>
-        <v>17289.614197050938</v>
+        <v>19331.587642070772</v>
       </c>
       <c r="N81" s="1">
         <f t="shared" si="4"/>
-        <v>17289.614197050938</v>
+        <v>19331.587642070772</v>
       </c>
     </row>
     <row r="82" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I82" s="1">
-        <f t="shared" si="2"/>
-        <v>84.294117647058783</v>
-      </c>
-      <c r="J82" s="1">
+      <c r="I82" s="36">
+        <f t="shared" si="2"/>
+        <v>93.549019607843078</v>
+      </c>
+      <c r="J82" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I82,$H$5,$H$6)/1000</f>
         <v>0</v>
       </c>
-      <c r="K82" s="1">
+      <c r="K82" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I82,$H$5,$H$6)</f>
         <v>0</v>
       </c>
       <c r="L82" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I82,$C$20,$H$5,$H$6)</f>
-        <v>17627.680677787979</v>
+        <v>19661.297400586489</v>
       </c>
       <c r="M82" s="1">
         <f t="shared" si="3"/>
-        <v>17627.680677787979</v>
+        <v>19661.297400586489</v>
       </c>
       <c r="N82" s="1">
         <f t="shared" si="4"/>
-        <v>17627.680677787979</v>
+        <v>19661.297400586489</v>
       </c>
     </row>
     <row r="83" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I83" s="1">
-        <f t="shared" si="2"/>
-        <v>85.705882352941131</v>
-      </c>
-      <c r="J83" s="1">
+      <c r="I83" s="36">
+        <f t="shared" si="2"/>
+        <v>95.117647058823465</v>
+      </c>
+      <c r="J83" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I83,$H$5,$H$6)/1000</f>
         <v>0</v>
       </c>
-      <c r="K83" s="1">
+      <c r="K83" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I83,$H$5,$H$6)</f>
         <v>0</v>
       </c>
       <c r="L83" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I83,$C$20,$H$5,$H$6)</f>
-        <v>17957.346134896223</v>
+        <v>19990.962848889663</v>
       </c>
       <c r="M83" s="1">
         <f t="shared" si="3"/>
-        <v>17957.346134896223</v>
+        <v>19990.962848889663</v>
       </c>
       <c r="N83" s="1">
         <f t="shared" si="4"/>
-        <v>17957.346134896223</v>
+        <v>19990.962848889663</v>
       </c>
     </row>
     <row r="84" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I84" s="1">
-        <f t="shared" si="2"/>
-        <v>87.117647058823479</v>
-      </c>
-      <c r="J84" s="1">
+      <c r="I84" s="36">
+        <f t="shared" si="2"/>
+        <v>96.686274509803852</v>
+      </c>
+      <c r="J84" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I84,$H$5,$H$6)/1000</f>
         <v>0</v>
       </c>
-      <c r="K84" s="1">
+      <c r="K84" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I84,$H$5,$H$6)</f>
         <v>0</v>
       </c>
       <c r="L84" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I84,$C$20,$H$5,$H$6)</f>
-        <v>18278.854772828065</v>
+        <v>20320.6968194492</v>
       </c>
       <c r="M84" s="1">
         <f t="shared" si="3"/>
-        <v>18278.854772828065</v>
+        <v>20320.6968194492</v>
       </c>
       <c r="N84" s="1">
         <f t="shared" si="4"/>
-        <v>18278.854772828065</v>
+        <v>20320.6968194492</v>
       </c>
     </row>
     <row r="85" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I85" s="1">
-        <f t="shared" si="2"/>
-        <v>88.529411764705827</v>
-      </c>
-      <c r="J85" s="1">
+      <c r="I85" s="36">
+        <f t="shared" si="2"/>
+        <v>98.254901960784238</v>
+      </c>
+      <c r="J85" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I85,$H$5,$H$6)/1000</f>
         <v>0</v>
       </c>
-      <c r="K85" s="1">
+      <c r="K85" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I85,$H$5,$H$6)</f>
         <v>0</v>
       </c>
       <c r="L85" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I85,$C$20,$H$5,$H$6)</f>
-        <v>18593.504749915024</v>
+        <v>20650.374634433319</v>
       </c>
       <c r="M85" s="1">
         <f t="shared" si="3"/>
-        <v>18593.504749915024</v>
+        <v>20650.374634433319</v>
       </c>
       <c r="N85" s="1">
         <f t="shared" si="4"/>
-        <v>18593.504749915024</v>
+        <v>20650.374634433319</v>
       </c>
     </row>
     <row r="86" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I86" s="1">
-        <f t="shared" si="2"/>
-        <v>89.941176470588175</v>
-      </c>
-      <c r="J86" s="1">
+      <c r="I86" s="36">
+        <f t="shared" si="2"/>
+        <v>99.823529411764625</v>
+      </c>
+      <c r="J86" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I86,$H$5,$H$6)/1000</f>
         <v>0</v>
       </c>
-      <c r="K86" s="1">
+      <c r="K86" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I86,$H$5,$H$6)</f>
         <v>0</v>
       </c>
       <c r="L86" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I86,$C$20,$H$5,$H$6)</f>
-        <v>18899.6877139922</v>
+        <v>20980.03300848497</v>
       </c>
       <c r="M86" s="1">
         <f t="shared" si="3"/>
-        <v>18899.6877139922</v>
+        <v>20980.03300848497</v>
       </c>
       <c r="N86" s="1">
         <f t="shared" si="4"/>
-        <v>18899.6877139922</v>
+        <v>20980.03300848497</v>
       </c>
     </row>
     <row r="87" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I87" s="1">
-        <f t="shared" si="2"/>
-        <v>91.352941176470523</v>
-      </c>
-      <c r="J87" s="1">
+      <c r="I87" s="36">
+        <f t="shared" si="2"/>
+        <v>101.39215686274501</v>
+      </c>
+      <c r="J87" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I87,$H$5,$H$6)/1000</f>
         <v>0</v>
       </c>
-      <c r="K87" s="1">
+      <c r="K87" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I87,$H$5,$H$6)</f>
         <v>0</v>
       </c>
       <c r="L87" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I87,$C$20,$H$5,$H$6)</f>
-        <v>19199.901980928051</v>
+        <v>21309.880987762608</v>
       </c>
       <c r="M87" s="1">
         <f t="shared" ref="M87:M99" si="5">IF(I87&gt;$C$40,L87,0)</f>
-        <v>19199.901980928051</v>
+        <v>21309.880987762608</v>
       </c>
       <c r="N87" s="1">
         <f t="shared" ref="N87:N99" si="6">IF(I87&gt;$C$39,L87,0)</f>
-        <v>19199.901980928051</v>
+        <v>21309.880987762608</v>
       </c>
     </row>
     <row r="88" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I88" s="1">
-        <f t="shared" si="2"/>
-        <v>92.764705882352871</v>
-      </c>
-      <c r="J88" s="1">
+      <c r="I88" s="36">
+        <f t="shared" si="2"/>
+        <v>102.9607843137254</v>
+      </c>
+      <c r="J88" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I88,$H$5,$H$6)/1000</f>
         <v>0</v>
       </c>
-      <c r="K88" s="1">
+      <c r="K88" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I88,$H$5,$H$6)</f>
         <v>0</v>
       </c>
       <c r="L88" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I88,$C$20,$H$5,$H$6)</f>
-        <v>19496.48142348669</v>
+        <v>21639.369247559269</v>
       </c>
       <c r="M88" s="1">
         <f t="shared" si="5"/>
-        <v>19496.48142348669</v>
+        <v>21639.369247559269</v>
       </c>
       <c r="N88" s="1">
         <f t="shared" si="6"/>
-        <v>19496.48142348669</v>
+        <v>21639.369247559269</v>
       </c>
     </row>
     <row r="89" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I89" s="1">
+      <c r="I89" s="36">
         <f t="shared" ref="I89:I99" si="7">I88+$I$21/51</f>
-        <v>94.176470588235219</v>
-      </c>
-      <c r="J89" s="1">
+        <v>104.52941176470578</v>
+      </c>
+      <c r="J89" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I89,$H$5,$H$6)/1000</f>
         <v>0</v>
       </c>
-      <c r="K89" s="1">
+      <c r="K89" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I89,$H$5,$H$6)</f>
         <v>0</v>
       </c>
       <c r="L89" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I89,$C$20,$H$5,$H$6)</f>
-        <v>19793.154075247352</v>
+        <v>21969.064307696721</v>
       </c>
       <c r="M89" s="1">
         <f t="shared" si="5"/>
-        <v>19793.154075247352</v>
+        <v>21969.064307696721</v>
       </c>
       <c r="N89" s="1">
         <f t="shared" si="6"/>
-        <v>19793.154075247352</v>
+        <v>21969.064307696721</v>
       </c>
     </row>
     <row r="90" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I90" s="1">
+      <c r="I90" s="36">
         <f t="shared" si="7"/>
-        <v>95.588235294117567</v>
-      </c>
-      <c r="J90" s="1">
+        <v>106.09803921568617</v>
+      </c>
+      <c r="J90" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I90,$H$5,$H$6)/1000</f>
         <v>0</v>
       </c>
-      <c r="K90" s="1">
+      <c r="K90" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I90,$H$5,$H$6)</f>
         <v>0</v>
       </c>
       <c r="L90" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I90,$C$20,$H$5,$H$6)</f>
-        <v>20089.929004556132</v>
+        <v>22298.704013237257</v>
       </c>
       <c r="M90" s="1">
         <f t="shared" si="5"/>
-        <v>20089.929004556132</v>
+        <v>22298.704013237257</v>
       </c>
       <c r="N90" s="1">
         <f t="shared" si="6"/>
-        <v>20089.929004556132</v>
+        <v>22298.704013237257</v>
       </c>
     </row>
     <row r="91" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I91" s="1">
+      <c r="I91" s="36">
         <f t="shared" si="7"/>
-        <v>96.999999999999915</v>
-      </c>
-      <c r="J91" s="1">
+        <v>107.66666666666656</v>
+      </c>
+      <c r="J91" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I91,$H$5,$H$6)/1000</f>
         <v>0</v>
       </c>
-      <c r="K91" s="1">
+      <c r="K91" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I91,$H$5,$H$6)</f>
         <v>0</v>
       </c>
       <c r="L91" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I91,$C$20,$H$5,$H$6)</f>
-        <v>20386.596363812845</v>
+        <v>22628.438630814489</v>
       </c>
       <c r="M91" s="1">
         <f t="shared" si="5"/>
-        <v>20386.596363812845</v>
+        <v>22628.438630814489</v>
       </c>
       <c r="N91" s="1">
         <f t="shared" si="6"/>
-        <v>20386.596363812845</v>
+        <v>22628.438630814489</v>
       </c>
     </row>
     <row r="92" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I92" s="1">
+      <c r="I92" s="36">
         <f t="shared" si="7"/>
-        <v>98.411764705882263</v>
-      </c>
-      <c r="J92" s="1">
+        <v>109.23529411764694</v>
+      </c>
+      <c r="J92" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I92,$H$5,$H$6)/1000</f>
         <v>0</v>
       </c>
-      <c r="K92" s="1">
+      <c r="K92" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I92,$H$5,$H$6)</f>
         <v>0</v>
       </c>
       <c r="L92" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I92,$C$20,$H$5,$H$6)</f>
-        <v>20683.372066720633</v>
+        <v>22958.078409093803</v>
       </c>
       <c r="M92" s="1">
         <f t="shared" si="5"/>
-        <v>20683.372066720633</v>
+        <v>22958.078409093803</v>
       </c>
       <c r="N92" s="1">
         <f t="shared" si="6"/>
-        <v>20683.372066720633</v>
+        <v>22958.078409093803</v>
       </c>
     </row>
     <row r="93" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I93" s="1">
+      <c r="I93" s="36">
         <f t="shared" si="7"/>
-        <v>99.823529411764611</v>
-      </c>
-      <c r="J93" s="1">
+        <v>110.80392156862733</v>
+      </c>
+      <c r="J93" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I93,$H$5,$H$6)/1000</f>
         <v>0</v>
       </c>
-      <c r="K93" s="1">
+      <c r="K93" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I93,$H$5,$H$6)</f>
         <v>0</v>
       </c>
       <c r="L93" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I93,$C$20,$H$5,$H$6)</f>
-        <v>20980.03300848461</v>
+        <v>23287.754627111255</v>
       </c>
       <c r="M93" s="1">
         <f t="shared" si="5"/>
-        <v>20980.03300848461</v>
+        <v>23287.754627111255</v>
       </c>
       <c r="N93" s="1">
         <f t="shared" si="6"/>
-        <v>20980.03300848461</v>
+        <v>23287.754627111255</v>
       </c>
     </row>
     <row r="94" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I94" s="1">
+      <c r="I94" s="36">
         <f t="shared" si="7"/>
-        <v>101.23529411764696</v>
-      </c>
-      <c r="J94" s="1">
+        <v>112.37254901960772</v>
+      </c>
+      <c r="J94" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I94,$H$5,$H$6)/1000</f>
         <v>0</v>
       </c>
-      <c r="K94" s="1">
+      <c r="K94" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I94,$H$5,$H$6)</f>
         <v>0</v>
       </c>
       <c r="L94" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I94,$C$20,$H$5,$H$6)</f>
-        <v>21276.766733582681</v>
+        <v>23617.698911038358</v>
       </c>
       <c r="M94" s="1">
         <f t="shared" si="5"/>
-        <v>21276.766733582681</v>
+        <v>23617.698911038358</v>
       </c>
       <c r="N94" s="1">
         <f t="shared" si="6"/>
-        <v>21276.766733582681</v>
+        <v>23617.698911038358</v>
       </c>
     </row>
     <row r="95" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I95" s="1">
+      <c r="I95" s="36">
         <f t="shared" si="7"/>
-        <v>102.64705882352931</v>
-      </c>
-      <c r="J95" s="1">
+        <v>113.9411764705881</v>
+      </c>
+      <c r="J95" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I95,$H$5,$H$6)/1000</f>
         <v>0</v>
       </c>
-      <c r="K95" s="1">
+      <c r="K95" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I95,$H$5,$H$6)</f>
         <v>0</v>
       </c>
       <c r="L95" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I95,$C$20,$H$5,$H$6)</f>
-        <v>21573.469266751661</v>
+        <v>23947.226282077449</v>
       </c>
       <c r="M95" s="1">
         <f t="shared" si="5"/>
-        <v>21573.469266751661</v>
+        <v>23947.226282077449</v>
       </c>
       <c r="N95" s="1">
         <f t="shared" si="6"/>
-        <v>21573.469266751661</v>
+        <v>23947.226282077449</v>
       </c>
     </row>
     <row r="96" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I96" s="1">
+      <c r="I96" s="36">
         <f t="shared" si="7"/>
-        <v>104.05882352941165</v>
-      </c>
-      <c r="J96" s="1">
+        <v>115.50980392156849</v>
+      </c>
+      <c r="J96" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I96,$H$5,$H$6)/1000</f>
         <v>0</v>
       </c>
-      <c r="K96" s="1">
+      <c r="K96" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I96,$H$5,$H$6)</f>
         <v>0</v>
       </c>
       <c r="L96" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I96,$C$20,$H$5,$H$6)</f>
-        <v>21870.245663779282</v>
+        <v>24276.781302305331</v>
       </c>
       <c r="M96" s="1">
         <f t="shared" si="5"/>
-        <v>21870.245663779282</v>
+        <v>24276.781302305331</v>
       </c>
       <c r="N96" s="1">
         <f t="shared" si="6"/>
-        <v>21870.245663779282</v>
+        <v>24276.781302305331</v>
       </c>
     </row>
     <row r="97" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I97" s="1">
+      <c r="I97" s="36">
         <f t="shared" si="7"/>
-        <v>105.470588235294</v>
-      </c>
-      <c r="J97" s="1">
+        <v>117.07843137254888</v>
+      </c>
+      <c r="J97" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I97,$H$5,$H$6)/1000</f>
         <v>0</v>
       </c>
-      <c r="K97" s="1">
+      <c r="K97" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I97,$H$5,$H$6)</f>
         <v>0</v>
       </c>
       <c r="L97" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I97,$C$20,$H$5,$H$6)</f>
-        <v>22166.875820776397</v>
+        <v>24606.48127580763</v>
       </c>
       <c r="M97" s="1">
         <f t="shared" si="5"/>
-        <v>22166.875820776397</v>
+        <v>24606.48127580763</v>
       </c>
       <c r="N97" s="1">
         <f t="shared" si="6"/>
-        <v>22166.875820776397</v>
+        <v>24606.48127580763</v>
       </c>
     </row>
     <row r="98" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I98" s="1">
+      <c r="I98" s="36">
         <f t="shared" si="7"/>
-        <v>106.88235294117635</v>
-      </c>
-      <c r="J98" s="1">
+        <v>118.64705882352926</v>
+      </c>
+      <c r="J98" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I98,$H$5,$H$6)/1000</f>
         <v>0</v>
       </c>
-      <c r="K98" s="1">
+      <c r="K98" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I98,$H$5,$H$6)</f>
         <v>0</v>
       </c>
       <c r="L98" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I98,$C$20,$H$5,$H$6)</f>
-        <v>22463.773442080615</v>
+        <v>24936.192523818027</v>
       </c>
       <c r="M98" s="1">
         <f t="shared" si="5"/>
-        <v>22463.773442080615</v>
+        <v>24936.192523818027</v>
       </c>
       <c r="N98" s="1">
         <f t="shared" si="6"/>
-        <v>22463.773442080615</v>
+        <v>24936.192523818027</v>
       </c>
     </row>
     <row r="99" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I99" s="1">
+      <c r="I99" s="36">
         <f t="shared" si="7"/>
-        <v>108.2941176470587</v>
-      </c>
-      <c r="J99" s="1">
+        <v>120.21568627450965</v>
+      </c>
+      <c r="J99" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I99,$H$5,$H$6)/1000</f>
         <v>0</v>
       </c>
-      <c r="K99" s="1">
+      <c r="K99" s="36">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,$C$19,I99,$H$5,$H$6)</f>
         <v>0</v>
       </c>
       <c r="L99" s="1">
         <f>[1]!GLV_q_gas_vkr_sm3day($C$12,$C$17,I99,$C$20,$H$5,$H$6)</f>
-        <v>22760.290125397136</v>
+        <v>25265.959124733825</v>
       </c>
       <c r="M99" s="1">
         <f t="shared" si="5"/>
-        <v>22760.290125397136</v>
+        <v>25265.959124733825</v>
       </c>
       <c r="N99" s="1">
         <f t="shared" si="6"/>
-        <v>22760.290125397136</v>
+        <v>25265.959124733825</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C11:D11"/>
@@ -5400,6 +5392,11 @@
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
   </mergeCells>
   <conditionalFormatting sqref="C5:D5">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="lessThanOrEqual">

</xml_diff>